<commit_message>
more analyses in data spreadsheet
</commit_message>
<xml_diff>
--- a/analyses/data-updated.xlsx
+++ b/analyses/data-updated.xlsx
@@ -424,7 +424,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -458,6 +458,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1668,10 +1669,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N70"/>
+  <dimension ref="A1:N67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="J38" sqref="J38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2625,32 +2626,34 @@
       <c r="B32" t="s">
         <v>61</v>
       </c>
-      <c r="C32" s="10">
+      <c r="C32" s="4">
         <v>415</v>
       </c>
-      <c r="D32" s="10">
+      <c r="D32" s="4">
         <v>2708</v>
       </c>
-      <c r="E32" s="10">
+      <c r="E32" s="4">
         <v>389</v>
       </c>
-      <c r="F32" s="10">
+      <c r="F32" s="4">
         <v>6</v>
       </c>
-      <c r="G32" s="10">
+      <c r="G32" s="4">
         <v>3</v>
       </c>
       <c r="H32" s="10">
         <v>0</v>
       </c>
-      <c r="I32" s="10"/>
-      <c r="J32" s="10">
+      <c r="I32" s="4">
+        <v>621</v>
+      </c>
+      <c r="J32" s="4">
         <v>78</v>
       </c>
-      <c r="K32" s="10">
+      <c r="K32" s="4">
         <v>226</v>
       </c>
-      <c r="L32" s="10">
+      <c r="L32" s="4">
         <v>449</v>
       </c>
       <c r="M32" s="10">
@@ -2667,7 +2670,7 @@
       <c r="D33" s="10">
         <v>0</v>
       </c>
-      <c r="E33" s="10">
+      <c r="E33" s="23">
         <v>3</v>
       </c>
       <c r="F33" s="10">
@@ -2679,7 +2682,9 @@
       <c r="H33" s="10">
         <v>0</v>
       </c>
-      <c r="I33" s="10"/>
+      <c r="I33" s="10">
+        <v>0</v>
+      </c>
       <c r="J33" s="10">
         <v>0</v>
       </c>
@@ -2694,23 +2699,23 @@
       </c>
     </row>
     <row r="34" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C34" s="13">
+      <c r="C34" s="14">
         <f t="shared" ref="C34:M34" si="5">SUM(C32:C33)</f>
         <v>415</v>
       </c>
-      <c r="D34" s="13">
+      <c r="D34" s="14">
         <f t="shared" si="5"/>
         <v>2708</v>
       </c>
-      <c r="E34" s="12">
+      <c r="E34" s="29">
         <f t="shared" si="5"/>
         <v>392</v>
       </c>
-      <c r="F34" s="13">
+      <c r="F34" s="14">
         <f t="shared" si="5"/>
         <v>6</v>
       </c>
-      <c r="G34" s="13">
+      <c r="G34" s="14">
         <f t="shared" si="5"/>
         <v>3</v>
       </c>
@@ -2718,15 +2723,19 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="J34" s="13">
+      <c r="I34" s="14">
+        <f>SUM(I32:I33)</f>
+        <v>621</v>
+      </c>
+      <c r="J34" s="14">
         <f t="shared" si="5"/>
         <v>78</v>
       </c>
-      <c r="K34" s="13">
+      <c r="K34" s="14">
         <f t="shared" si="5"/>
         <v>226</v>
       </c>
-      <c r="L34" s="13">
+      <c r="L34" s="14">
         <f t="shared" si="5"/>
         <v>449</v>
       </c>
@@ -2737,540 +2746,547 @@
     </row>
     <row r="35" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+      <c r="C36" s="10"/>
+      <c r="D36" s="10"/>
+      <c r="E36" s="10"/>
+      <c r="F36" s="10"/>
+      <c r="G36" s="10"/>
+      <c r="H36" s="10"/>
+      <c r="I36" s="10"/>
+      <c r="J36" s="10"/>
+      <c r="K36" s="10"/>
+      <c r="L36" s="10"/>
+      <c r="M36" s="10"/>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>85</v>
+      </c>
+      <c r="B37" t="s">
+        <v>84</v>
+      </c>
+      <c r="C37" s="10">
+        <v>0</v>
+      </c>
+      <c r="D37" s="4">
+        <v>1</v>
+      </c>
+      <c r="E37" s="4">
+        <v>8</v>
+      </c>
+      <c r="F37" s="10">
+        <v>0</v>
+      </c>
+      <c r="G37" s="10">
+        <v>0</v>
+      </c>
+      <c r="H37" s="10">
+        <v>0</v>
+      </c>
+      <c r="I37" s="4">
+        <v>1</v>
+      </c>
+      <c r="J37" s="10">
+        <v>0</v>
+      </c>
+      <c r="K37" s="10">
+        <v>0</v>
+      </c>
+      <c r="L37" s="10">
+        <v>0</v>
+      </c>
+      <c r="M37" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C38" s="10"/>
+      <c r="D38" s="10"/>
+      <c r="E38" s="10"/>
+      <c r="F38" s="10"/>
+      <c r="G38" s="10"/>
+      <c r="H38" s="10"/>
+      <c r="I38" s="10"/>
+      <c r="J38" s="10"/>
+      <c r="K38" s="10"/>
+      <c r="L38" s="10"/>
+      <c r="M38" s="10"/>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>86</v>
+      </c>
+      <c r="B39" t="s">
+        <v>87</v>
+      </c>
+      <c r="C39" s="10">
+        <v>0</v>
+      </c>
+      <c r="D39" s="7">
+        <v>4</v>
+      </c>
+      <c r="E39" s="7">
+        <v>5</v>
+      </c>
+      <c r="F39" s="10">
+        <v>0</v>
+      </c>
+      <c r="G39" s="10">
+        <v>0</v>
+      </c>
+      <c r="H39" s="10">
+        <v>0</v>
+      </c>
+      <c r="I39" s="7">
+        <v>8</v>
+      </c>
+      <c r="J39" s="10">
+        <v>0</v>
+      </c>
+      <c r="K39" s="7">
+        <v>64</v>
+      </c>
+      <c r="L39" s="10">
+        <v>0</v>
+      </c>
+      <c r="M39" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C40" s="10"/>
+      <c r="D40" s="10"/>
+      <c r="E40" s="10"/>
+      <c r="F40" s="10"/>
+      <c r="G40" s="10"/>
+      <c r="H40" s="10"/>
+      <c r="I40" s="10"/>
+      <c r="J40" s="10"/>
+      <c r="K40" s="10"/>
+      <c r="L40" s="10"/>
+      <c r="M40" s="10"/>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>88</v>
+      </c>
+      <c r="B41" t="s">
+        <v>89</v>
+      </c>
+      <c r="C41" s="4">
+        <v>1</v>
+      </c>
+      <c r="D41" s="4">
+        <v>2</v>
+      </c>
+      <c r="E41" s="4">
+        <v>6</v>
+      </c>
+      <c r="F41" s="4">
+        <v>2</v>
+      </c>
+      <c r="G41" s="10">
+        <v>0</v>
+      </c>
+      <c r="H41" s="10">
+        <v>0</v>
+      </c>
+      <c r="I41" s="4">
+        <v>15</v>
+      </c>
+      <c r="J41" s="10">
+        <v>0</v>
+      </c>
+      <c r="K41" s="4">
+        <v>19</v>
+      </c>
+      <c r="L41" s="10">
+        <v>0</v>
+      </c>
+      <c r="M41" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C42" s="10"/>
+      <c r="D42" s="10"/>
+      <c r="E42" s="10"/>
+      <c r="F42" s="10"/>
+      <c r="G42" s="10"/>
+      <c r="H42" s="10"/>
+      <c r="I42" s="10"/>
+      <c r="J42" s="10"/>
+      <c r="K42" s="10"/>
+      <c r="L42" s="10"/>
+      <c r="M42" s="10"/>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>91</v>
+      </c>
+      <c r="B43" t="s">
+        <v>90</v>
+      </c>
+      <c r="C43" s="10">
+        <v>0</v>
+      </c>
+      <c r="D43" s="4">
+        <v>17</v>
+      </c>
+      <c r="E43" s="10">
+        <v>0</v>
+      </c>
+      <c r="F43" s="10">
+        <v>0</v>
+      </c>
+      <c r="G43" s="10">
+        <v>0</v>
+      </c>
+      <c r="H43" s="10">
+        <v>0</v>
+      </c>
+      <c r="I43" s="4">
+        <v>20</v>
+      </c>
+      <c r="J43" s="10">
+        <v>0</v>
+      </c>
+      <c r="K43" s="4">
+        <v>1003</v>
+      </c>
+      <c r="L43" s="4">
+        <v>14</v>
+      </c>
+      <c r="M43" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>92</v>
+      </c>
+      <c r="C44" s="4">
+        <v>147</v>
+      </c>
+      <c r="D44" s="4">
+        <v>7</v>
+      </c>
+      <c r="E44" s="4">
+        <v>191</v>
+      </c>
+      <c r="F44" s="4">
+        <v>37</v>
+      </c>
+      <c r="G44" s="4">
+        <v>1</v>
+      </c>
+      <c r="H44" s="10">
+        <v>0</v>
+      </c>
+      <c r="I44" s="4">
+        <v>157</v>
+      </c>
+      <c r="J44" s="10">
+        <v>0</v>
+      </c>
+      <c r="K44" s="4">
+        <v>932</v>
+      </c>
+      <c r="L44" s="4">
+        <v>40</v>
+      </c>
+      <c r="M44" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C45" s="14">
+        <f>SUM(C43:C44)</f>
+        <v>147</v>
+      </c>
+      <c r="D45" s="14">
+        <f>SUM(D43:D44)</f>
+        <v>24</v>
+      </c>
+      <c r="E45" s="14">
+        <f>SUM(E43:E44)</f>
+        <v>191</v>
+      </c>
+      <c r="F45" s="14">
+        <f>SUM(F43:F44)</f>
+        <v>37</v>
+      </c>
+      <c r="G45" s="14">
+        <f>SUM(G43:G44)</f>
+        <v>1</v>
+      </c>
+      <c r="H45" s="13">
+        <f t="shared" ref="C45:H45" si="6">SUM(H43:H44)</f>
+        <v>0</v>
+      </c>
+      <c r="I45" s="14">
+        <f>SUM(I43:I44)</f>
+        <v>177</v>
+      </c>
+      <c r="J45" s="13">
+        <f>SUM(J43:J44)</f>
+        <v>0</v>
+      </c>
+      <c r="K45" s="14">
+        <f>SUM(K43:K44)</f>
+        <v>1935</v>
+      </c>
+      <c r="L45" s="14">
+        <f>SUM(L43:L44)</f>
+        <v>54</v>
+      </c>
+      <c r="M45" s="13">
+        <f>SUM(M43:M44)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C46" s="10"/>
+      <c r="D46" s="10"/>
+      <c r="E46" s="10"/>
+      <c r="F46" s="10"/>
+      <c r="G46" s="10"/>
+      <c r="H46" s="10"/>
+      <c r="I46" s="10"/>
+      <c r="J46" s="10"/>
+      <c r="K46" s="10"/>
+      <c r="L46" s="10"/>
+      <c r="M46" s="10"/>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>93</v>
+      </c>
+      <c r="B47" t="s">
+        <v>94</v>
+      </c>
+      <c r="C47" s="4">
+        <v>3</v>
+      </c>
+      <c r="D47" s="10">
+        <v>0</v>
+      </c>
+      <c r="E47" s="4">
+        <v>6</v>
+      </c>
+      <c r="F47" s="10">
+        <v>0</v>
+      </c>
+      <c r="G47" s="10">
+        <v>0</v>
+      </c>
+      <c r="H47" s="4">
+        <v>6</v>
+      </c>
+      <c r="I47" s="4">
+        <v>29</v>
+      </c>
+      <c r="J47" s="10">
+        <v>0</v>
+      </c>
+      <c r="K47" s="4">
+        <v>41</v>
+      </c>
+      <c r="L47" s="4">
+        <v>4</v>
+      </c>
+      <c r="M47" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>95</v>
+      </c>
+      <c r="C48" s="4">
+        <v>14</v>
+      </c>
+      <c r="D48" s="4">
+        <v>2</v>
+      </c>
+      <c r="E48" s="7">
+        <v>244</v>
+      </c>
+      <c r="F48" s="10">
+        <v>0</v>
+      </c>
+      <c r="G48" s="10">
+        <v>0</v>
+      </c>
+      <c r="H48" s="7">
+        <v>42</v>
+      </c>
+      <c r="I48" s="7">
+        <v>61</v>
+      </c>
+      <c r="J48" s="10">
+        <v>0</v>
+      </c>
+      <c r="K48" s="4">
+        <v>5</v>
+      </c>
+      <c r="L48" s="10">
+        <v>0</v>
+      </c>
+      <c r="M48" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>33</v>
+      </c>
+      <c r="C49" s="14">
+        <v>5</v>
+      </c>
+      <c r="D49" s="14">
+        <v>0</v>
+      </c>
+      <c r="E49" s="15">
+        <v>9</v>
+      </c>
+      <c r="F49" s="13">
+        <v>0</v>
+      </c>
+      <c r="G49" s="13">
+        <v>0</v>
+      </c>
+      <c r="H49" s="15">
+        <v>44</v>
+      </c>
+      <c r="I49" s="15">
+        <f>SUM(I47:I48)</f>
+        <v>90</v>
+      </c>
+      <c r="J49" s="13">
+        <v>0</v>
+      </c>
+      <c r="K49" s="14">
+        <v>4</v>
+      </c>
+      <c r="L49" s="13">
+        <v>0</v>
+      </c>
+      <c r="M49" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
         <v>63</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B52" t="s">
         <v>64</v>
       </c>
-      <c r="C36" s="10">
+      <c r="C52" s="10">
         <v>118</v>
       </c>
-      <c r="D36" s="10">
+      <c r="D52" s="10">
         <v>420</v>
       </c>
-      <c r="E36" s="10">
+      <c r="E52" s="10">
         <v>188</v>
       </c>
-      <c r="F36" s="10">
+      <c r="F52" s="10">
         <v>2</v>
       </c>
-      <c r="G36" s="10">
+      <c r="G52" s="10">
         <v>8</v>
       </c>
-      <c r="H36" s="10">
-        <v>0</v>
-      </c>
-      <c r="I36" s="10"/>
-      <c r="J36" s="10">
-        <v>0</v>
-      </c>
-      <c r="K36" s="10">
-        <v>297</v>
-      </c>
-      <c r="L36" s="10">
-        <v>9</v>
-      </c>
-      <c r="M36" s="10">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C37" s="10"/>
-      <c r="D37" s="10"/>
-      <c r="E37" s="10"/>
-      <c r="F37" s="10"/>
-      <c r="G37" s="10"/>
-      <c r="H37" s="10"/>
-      <c r="I37" s="10"/>
-      <c r="J37" s="10"/>
-      <c r="K37" s="10"/>
-      <c r="L37" s="10"/>
-      <c r="M37" s="10"/>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>83</v>
-      </c>
-      <c r="B38" t="s">
-        <v>82</v>
-      </c>
-      <c r="C38" s="10">
-        <v>13</v>
-      </c>
-      <c r="D38" s="10">
-        <v>116</v>
-      </c>
-      <c r="E38" s="10">
-        <v>143</v>
-      </c>
-      <c r="F38" s="10">
-        <v>0</v>
-      </c>
-      <c r="G38" s="10">
-        <v>0</v>
-      </c>
-      <c r="H38" s="10">
-        <v>0</v>
-      </c>
-      <c r="I38" s="10"/>
-      <c r="J38" s="10">
-        <v>0</v>
-      </c>
-      <c r="K38" s="10">
-        <v>209</v>
-      </c>
-      <c r="L38" s="10">
-        <v>1</v>
-      </c>
-      <c r="M38" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C39" s="10"/>
-      <c r="D39" s="10"/>
-      <c r="E39" s="10"/>
-      <c r="F39" s="10"/>
-      <c r="G39" s="10"/>
-      <c r="H39" s="10"/>
-      <c r="I39" s="10"/>
-      <c r="J39" s="10"/>
-      <c r="K39" s="10"/>
-      <c r="L39" s="10"/>
-      <c r="M39" s="10"/>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>85</v>
-      </c>
-      <c r="B40" t="s">
-        <v>84</v>
-      </c>
-      <c r="C40" s="10">
-        <v>0</v>
-      </c>
-      <c r="D40" s="10">
-        <v>2</v>
-      </c>
-      <c r="E40" s="10">
-        <v>10</v>
-      </c>
-      <c r="F40" s="10">
-        <v>0</v>
-      </c>
-      <c r="G40" s="10">
-        <v>0</v>
-      </c>
-      <c r="H40" s="10">
-        <v>0</v>
-      </c>
-      <c r="I40" s="10"/>
-      <c r="J40" s="10">
-        <v>0</v>
-      </c>
-      <c r="K40" s="10">
-        <v>0</v>
-      </c>
-      <c r="L40" s="10">
-        <v>0</v>
-      </c>
-      <c r="M40" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C41" s="10"/>
-      <c r="D41" s="10"/>
-      <c r="E41" s="10"/>
-      <c r="F41" s="10"/>
-      <c r="G41" s="10"/>
-      <c r="H41" s="10"/>
-      <c r="I41" s="10"/>
-      <c r="J41" s="10"/>
-      <c r="K41" s="10"/>
-      <c r="L41" s="10"/>
-      <c r="M41" s="10"/>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>86</v>
-      </c>
-      <c r="B42" t="s">
-        <v>87</v>
-      </c>
-      <c r="C42" s="10">
-        <v>0</v>
-      </c>
-      <c r="D42" s="10">
-        <v>4</v>
-      </c>
-      <c r="E42" s="10">
-        <v>5</v>
-      </c>
-      <c r="F42" s="10">
-        <v>0</v>
-      </c>
-      <c r="G42" s="10">
-        <v>0</v>
-      </c>
-      <c r="H42" s="10">
-        <v>0</v>
-      </c>
-      <c r="I42" s="10"/>
-      <c r="J42" s="10">
-        <v>0</v>
-      </c>
-      <c r="K42" s="10">
-        <v>64</v>
-      </c>
-      <c r="L42" s="10">
-        <v>0</v>
-      </c>
-      <c r="M42" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C43" s="10"/>
-      <c r="D43" s="10"/>
-      <c r="E43" s="10"/>
-      <c r="F43" s="10"/>
-      <c r="G43" s="10"/>
-      <c r="H43" s="10"/>
-      <c r="I43" s="10"/>
-      <c r="J43" s="10"/>
-      <c r="K43" s="10"/>
-      <c r="L43" s="10"/>
-      <c r="M43" s="10"/>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>88</v>
-      </c>
-      <c r="B44" t="s">
-        <v>89</v>
-      </c>
-      <c r="C44" s="10">
-        <v>1</v>
-      </c>
-      <c r="D44" s="10">
-        <v>2</v>
-      </c>
-      <c r="E44" s="10">
-        <v>6</v>
-      </c>
-      <c r="F44" s="10">
-        <v>2</v>
-      </c>
-      <c r="G44" s="10">
-        <v>0</v>
-      </c>
-      <c r="H44" s="10">
-        <v>0</v>
-      </c>
-      <c r="I44" s="10"/>
-      <c r="J44" s="10">
-        <v>0</v>
-      </c>
-      <c r="K44" s="10">
-        <v>19</v>
-      </c>
-      <c r="L44" s="10">
-        <v>0</v>
-      </c>
-      <c r="M44" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C45" s="10"/>
-      <c r="D45" s="10"/>
-      <c r="E45" s="10"/>
-      <c r="F45" s="10"/>
-      <c r="G45" s="10"/>
-      <c r="H45" s="10"/>
-      <c r="I45" s="10"/>
-      <c r="J45" s="10"/>
-      <c r="K45" s="10"/>
-      <c r="L45" s="10"/>
-      <c r="M45" s="10"/>
-    </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>91</v>
-      </c>
-      <c r="B46" t="s">
-        <v>90</v>
-      </c>
-      <c r="C46" s="10">
-        <v>0</v>
-      </c>
-      <c r="D46" s="10">
-        <v>17</v>
-      </c>
-      <c r="E46" s="10">
-        <v>0</v>
-      </c>
-      <c r="F46" s="10">
-        <v>0</v>
-      </c>
-      <c r="G46" s="10">
-        <v>0</v>
-      </c>
-      <c r="H46" s="10">
-        <v>0</v>
-      </c>
-      <c r="I46" s="10"/>
-      <c r="J46" s="10">
-        <v>0</v>
-      </c>
-      <c r="K46" s="10">
-        <v>1003</v>
-      </c>
-      <c r="L46" s="10">
-        <v>14</v>
-      </c>
-      <c r="M46" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B47" t="s">
-        <v>92</v>
-      </c>
-      <c r="C47" s="10">
-        <v>147</v>
-      </c>
-      <c r="D47" s="10">
-        <v>7</v>
-      </c>
-      <c r="E47" s="10">
-        <v>191</v>
-      </c>
-      <c r="F47" s="10">
-        <v>37</v>
-      </c>
-      <c r="G47" s="10">
-        <v>1</v>
-      </c>
-      <c r="H47" s="10">
-        <v>0</v>
-      </c>
-      <c r="I47" s="10"/>
-      <c r="J47" s="10">
-        <v>0</v>
-      </c>
-      <c r="K47" s="10">
-        <v>932</v>
-      </c>
-      <c r="L47" s="10">
-        <v>40</v>
-      </c>
-      <c r="M47" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C48" s="10">
-        <f>SUM(C46:C47)</f>
-        <v>147</v>
-      </c>
-      <c r="D48" s="10">
-        <f>SUM(D46:D47)</f>
-        <v>24</v>
-      </c>
-      <c r="E48" s="10">
-        <f>SUM(E46:E47)</f>
-        <v>191</v>
-      </c>
-      <c r="F48" s="10">
-        <f>SUM(F46:F47)</f>
-        <v>37</v>
-      </c>
-      <c r="G48" s="10">
-        <f>SUM(G46:G47)</f>
-        <v>1</v>
-      </c>
-      <c r="H48" s="10">
-        <f>SUM(H46:H47)</f>
-        <v>0</v>
-      </c>
-      <c r="I48" s="10"/>
-      <c r="J48" s="10">
-        <f>SUM(J46:J47)</f>
-        <v>0</v>
-      </c>
-      <c r="K48" s="10">
-        <f>SUM(K46:K47)</f>
-        <v>1935</v>
-      </c>
-      <c r="L48" s="10">
-        <f>SUM(L46:L47)</f>
-        <v>54</v>
-      </c>
-      <c r="M48" s="10">
-        <f>SUM(M46:M47)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C49" s="10"/>
-      <c r="D49" s="10"/>
-      <c r="E49" s="10"/>
-      <c r="F49" s="10"/>
-      <c r="G49" s="10"/>
-      <c r="H49" s="10"/>
-      <c r="I49" s="10"/>
-      <c r="J49" s="10"/>
-      <c r="K49" s="10"/>
-      <c r="L49" s="10"/>
-      <c r="M49" s="10"/>
-    </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>93</v>
-      </c>
-      <c r="B50" t="s">
-        <v>94</v>
-      </c>
-      <c r="C50" s="10">
-        <v>3</v>
-      </c>
-      <c r="D50" s="10">
-        <v>0</v>
-      </c>
-      <c r="E50" s="10">
-        <v>6</v>
-      </c>
-      <c r="F50" s="10">
-        <v>0</v>
-      </c>
-      <c r="G50" s="10">
-        <v>0</v>
-      </c>
-      <c r="H50" s="10">
-        <v>6</v>
-      </c>
-      <c r="I50" s="10"/>
-      <c r="J50" s="10">
-        <v>0</v>
-      </c>
-      <c r="K50" s="10">
-        <v>41</v>
-      </c>
-      <c r="L50" s="10">
-        <v>4</v>
-      </c>
-      <c r="M50" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B51" t="s">
-        <v>95</v>
-      </c>
-      <c r="C51" s="10">
-        <v>14</v>
-      </c>
-      <c r="D51" s="10">
-        <v>2</v>
-      </c>
-      <c r="E51" s="10">
-        <v>246</v>
-      </c>
-      <c r="F51" s="10">
-        <v>0</v>
-      </c>
-      <c r="G51" s="10">
-        <v>0</v>
-      </c>
-      <c r="H51" s="10">
-        <v>43</v>
-      </c>
-      <c r="I51" s="10"/>
-      <c r="J51" s="10">
-        <v>0</v>
-      </c>
-      <c r="K51" s="10">
-        <v>5</v>
-      </c>
-      <c r="L51" s="10">
-        <v>0</v>
-      </c>
-      <c r="M51" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B52" t="s">
-        <v>33</v>
-      </c>
-      <c r="C52" s="10">
-        <v>5</v>
-      </c>
-      <c r="D52" s="10">
-        <v>0</v>
-      </c>
-      <c r="E52" s="10">
-        <v>9</v>
-      </c>
-      <c r="F52" s="10">
-        <v>0</v>
-      </c>
-      <c r="G52" s="10">
-        <v>0</v>
-      </c>
       <c r="H52" s="10">
-        <v>44</v>
+        <v>0</v>
       </c>
       <c r="I52" s="10"/>
       <c r="J52" s="10">
         <v>0</v>
       </c>
       <c r="K52" s="10">
-        <v>4</v>
+        <v>297</v>
       </c>
       <c r="L52" s="10">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="M52" s="10">
-        <v>0</v>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>83</v>
+      </c>
+      <c r="B53" t="s">
+        <v>82</v>
+      </c>
+      <c r="C53" s="10">
+        <v>13</v>
+      </c>
+      <c r="D53" s="10">
+        <v>116</v>
+      </c>
+      <c r="E53" s="10">
+        <v>143</v>
+      </c>
+      <c r="F53" s="10">
+        <v>0</v>
+      </c>
+      <c r="G53" s="10">
+        <v>0</v>
+      </c>
+      <c r="H53" s="10">
+        <v>0</v>
+      </c>
+      <c r="I53" s="10"/>
+      <c r="J53" s="10">
+        <v>0</v>
+      </c>
+      <c r="K53" s="10">
+        <v>209</v>
+      </c>
+      <c r="L53" s="10">
+        <v>1</v>
+      </c>
+      <c r="M53" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A60" s="5"/>
+      <c r="B60" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A61" s="6"/>
+      <c r="B61" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A62" s="8"/>
+      <c r="B62" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A63" s="5"/>
+      <c r="A63" s="7"/>
       <c r="B63" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A64" s="6"/>
+      <c r="A64" s="4"/>
       <c r="B64" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="8"/>
-      <c r="B65" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" s="7"/>
-      <c r="B66" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" s="4"/>
+      <c r="A67" s="9"/>
       <c r="B67" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" s="9"/>
-      <c r="B70" t="s">
         <v>98</v>
       </c>
     </row>

</xml_diff>

<commit_message>
making sure repo up to date
</commit_message>
<xml_diff>
--- a/analyses/data-updated.xlsx
+++ b/analyses/data-updated.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="30" windowWidth="27795" windowHeight="13350" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15520" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="full values" sheetId="1" r:id="rId1"/>
@@ -15,12 +15,17 @@
     <sheet name="feature graph orderings" sheetId="8" r:id="rId6"/>
     <sheet name="Sheet5" sheetId="5" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="132">
   <si>
     <t>Developer</t>
   </si>
@@ -317,13 +322,112 @@
   </si>
   <si>
     <t>null not sure why!</t>
+  </si>
+  <si>
+    <t>novoda/spikes</t>
+  </si>
+  <si>
+    <t>novoda/merlin</t>
+  </si>
+  <si>
+    <t>novoda/landing-strip</t>
+  </si>
+  <si>
+    <t>ouchadam/lol-dr</t>
+  </si>
+  <si>
+    <t>iluwatar/java-design-patterns</t>
+  </si>
+  <si>
+    <t>laamella-gad/file-index</t>
+  </si>
+  <si>
+    <t>CIRDLES/MARS</t>
+  </si>
+  <si>
+    <t>jimbarritt</t>
+  </si>
+  <si>
+    <t>bugsim</t>
+  </si>
+  <si>
+    <t>cumulus-code</t>
+  </si>
+  <si>
+    <t>openam-oauth-scope-validators</t>
+  </si>
+  <si>
+    <t>jmdb-tutorial/neo4j-demo</t>
+  </si>
+  <si>
+    <t>ixcode/openam-server</t>
+  </si>
+  <si>
+    <t>jmdb-tutorial/web-security</t>
+  </si>
+  <si>
+    <t>akshaymankar</t>
+  </si>
+  <si>
+    <t>biblioteca</t>
+  </si>
+  <si>
+    <t>hugocorbucci</t>
+  </si>
+  <si>
+    <t>Editor-Switcher</t>
+  </si>
+  <si>
+    <t>SWT-Minesweeper</t>
+  </si>
+  <si>
+    <t>thejamesthomas</t>
+  </si>
+  <si>
+    <t>mountebank-maven-plugin</t>
+  </si>
+  <si>
+    <t>javabank</t>
+  </si>
+  <si>
+    <t>aj-jaswanth</t>
+  </si>
+  <si>
+    <t>openmrs-core</t>
+  </si>
+  <si>
+    <t>openmrs-module-bedmanagement</t>
+  </si>
+  <si>
+    <t>bahmni-reports</t>
+  </si>
+  <si>
+    <t>twu-biblioteca-jaswanth</t>
+  </si>
+  <si>
+    <t>sales-tax-2</t>
+  </si>
+  <si>
+    <t>hello-world</t>
+  </si>
+  <si>
+    <t>Sales-Tax-App</t>
+  </si>
+  <si>
+    <t>Game-Of-Life-New</t>
+  </si>
+  <si>
+    <t>phoenix-proxy-server</t>
+  </si>
+  <si>
+    <t>Bahmni/bahmni-reports</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -365,6 +469,28 @@
       <color rgb="FF00B050"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="6" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -421,10 +547,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -459,8 +593,18 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="9">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -766,27 +910,27 @@
       <selection activeCell="B1" sqref="B1:B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.5" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="9" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" s="2" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -842,7 +986,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -895,7 +1039,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -948,7 +1092,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20">
       <c r="B4" t="s">
         <v>19</v>
       </c>
@@ -998,7 +1142,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -1051,7 +1195,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20">
       <c r="B6" t="s">
         <v>22</v>
       </c>
@@ -1101,7 +1245,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -1154,7 +1298,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20">
       <c r="B8" t="s">
         <v>25</v>
       </c>
@@ -1204,7 +1348,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20">
       <c r="B9" t="s">
         <v>26</v>
       </c>
@@ -1254,7 +1398,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20">
       <c r="B10" t="s">
         <v>38</v>
       </c>
@@ -1301,7 +1445,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -1354,7 +1498,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20">
       <c r="B12" t="s">
         <v>31</v>
       </c>
@@ -1404,7 +1548,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20">
       <c r="B13" t="s">
         <v>36</v>
       </c>
@@ -1454,7 +1598,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20">
       <c r="A14" t="s">
         <v>32</v>
       </c>
@@ -1507,7 +1651,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20">
       <c r="B15" t="s">
         <v>34</v>
       </c>
@@ -1557,7 +1701,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20">
       <c r="B16" t="s">
         <v>35</v>
       </c>
@@ -1607,7 +1751,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="5:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="5:18">
       <c r="E19">
         <f>SUM(E2:E16)</f>
         <v>0</v>
@@ -1663,32 +1807,37 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="landscape" r:id="rId1"/>
+  <pageSetup orientation="landscape"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N67"/>
+  <dimension ref="A1:N112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="J38" sqref="J38"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="23" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1729,7 +1878,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14">
       <c r="A2" s="24" t="s">
         <v>15</v>
       </c>
@@ -1748,7 +1897,7 @@
       <c r="F2" s="8">
         <v>38</v>
       </c>
-      <c r="G2" s="8">
+      <c r="G2" s="10">
         <v>0</v>
       </c>
       <c r="H2" s="8">
@@ -1770,15 +1919,49 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" s="10" customFormat="1">
       <c r="A3" s="25"/>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="24" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" t="s">
-        <v>45</v>
+      <c r="B3" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="C3" s="10">
+        <v>0</v>
+      </c>
+      <c r="D3" s="10">
+        <v>0</v>
+      </c>
+      <c r="E3" s="7">
+        <v>2</v>
+      </c>
+      <c r="F3" s="10">
+        <v>0</v>
+      </c>
+      <c r="G3" s="10">
+        <v>0</v>
+      </c>
+      <c r="H3" s="10">
+        <v>0</v>
+      </c>
+      <c r="I3" s="10">
+        <v>0</v>
+      </c>
+      <c r="J3" s="10">
+        <v>0</v>
+      </c>
+      <c r="K3" s="10">
+        <v>0</v>
+      </c>
+      <c r="L3" s="10">
+        <v>0</v>
+      </c>
+      <c r="M3" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" s="10" customFormat="1">
+      <c r="A4" s="25"/>
+      <c r="B4" s="10" t="s">
+        <v>100</v>
       </c>
       <c r="C4" s="10">
         <v>0</v>
@@ -1786,8 +1969,8 @@
       <c r="D4" s="10">
         <v>0</v>
       </c>
-      <c r="E4" s="8">
-        <v>1</v>
+      <c r="E4" s="7">
+        <v>2</v>
       </c>
       <c r="F4" s="10">
         <v>0</v>
@@ -1798,7 +1981,9 @@
       <c r="H4" s="10">
         <v>0</v>
       </c>
-      <c r="I4" s="10"/>
+      <c r="I4" s="10">
+        <v>0</v>
+      </c>
       <c r="J4" s="10">
         <v>0</v>
       </c>
@@ -1812,59 +1997,58 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="24"/>
-      <c r="B5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="8">
-        <v>17</v>
-      </c>
-      <c r="D5" s="8">
-        <v>10</v>
+    <row r="5" spans="1:14" s="10" customFormat="1">
+      <c r="A5" s="25"/>
+      <c r="B5" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="C5" s="10">
+        <v>0</v>
+      </c>
+      <c r="D5" s="10">
+        <v>0</v>
       </c>
       <c r="E5" s="6">
-        <v>177</v>
-      </c>
-      <c r="F5" s="8">
-        <v>2</v>
+        <v>35</v>
+      </c>
+      <c r="F5" s="10">
+        <v>0</v>
       </c>
       <c r="G5" s="10">
         <v>0</v>
       </c>
-      <c r="H5" s="6">
-        <v>87</v>
-      </c>
-      <c r="I5" s="6">
-        <v>38</v>
+      <c r="H5" s="10">
+        <v>0</v>
+      </c>
+      <c r="I5" s="10">
+        <v>0</v>
       </c>
       <c r="J5" s="10">
         <v>0</v>
       </c>
-      <c r="K5" s="8">
-        <v>13</v>
-      </c>
-      <c r="L5" s="9">
-        <v>7</v>
-      </c>
-      <c r="M5" s="8">
-        <v>2</v>
-      </c>
-      <c r="N5" s="10"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="24"/>
-      <c r="B6" t="s">
-        <v>19</v>
+      <c r="K5" s="10">
+        <v>0</v>
+      </c>
+      <c r="L5" s="10">
+        <v>0</v>
+      </c>
+      <c r="M5" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" s="10" customFormat="1">
+      <c r="A6" s="25"/>
+      <c r="B6" s="10" t="s">
+        <v>102</v>
       </c>
       <c r="C6" s="7">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D6" s="10">
         <v>0</v>
       </c>
       <c r="E6" s="7">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="F6" s="7">
         <v>1</v>
@@ -1876,1423 +2060,1942 @@
         <v>0</v>
       </c>
       <c r="I6" s="7">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="J6" s="10">
         <v>0</v>
       </c>
       <c r="K6" s="7">
-        <v>3</v>
-      </c>
-      <c r="L6" s="10">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="L6" s="7">
+        <v>1</v>
       </c>
       <c r="M6" s="10">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:14" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" s="13" customFormat="1">
       <c r="A7" s="26"/>
       <c r="C7" s="16">
-        <f t="shared" ref="C7:M7" si="0">SUM(C4:C6)</f>
+        <f>SUM(C2:C6)</f>
+        <v>254</v>
+      </c>
+      <c r="D7" s="16">
+        <f>SUM(D2:D6)</f>
+        <v>37</v>
+      </c>
+      <c r="E7" s="27">
+        <f>SUM(E2:E6)</f>
+        <v>429</v>
+      </c>
+      <c r="F7" s="16">
+        <f>SUM(F2:F6)</f>
+        <v>39</v>
+      </c>
+      <c r="G7" s="13">
+        <f>SUM(G2:G6)</f>
+        <v>0</v>
+      </c>
+      <c r="H7" s="16">
+        <f>SUM(H2:H6)</f>
+        <v>27</v>
+      </c>
+      <c r="I7" s="16">
+        <f>SUM(I2:I6)</f>
+        <v>52</v>
+      </c>
+      <c r="J7" s="16">
+        <f>SUM(J2:J6)</f>
+        <v>3</v>
+      </c>
+      <c r="K7" s="16">
+        <f>SUM(K2:K6)</f>
+        <v>131</v>
+      </c>
+      <c r="L7" s="16">
+        <f>SUM(L2:L6)</f>
+        <v>70</v>
+      </c>
+      <c r="M7" s="13">
+        <f>SUM(M2:M6)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" s="10" customFormat="1">
+      <c r="A8" s="25"/>
+    </row>
+    <row r="9" spans="1:14">
+      <c r="A9" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" s="10">
+        <v>0</v>
+      </c>
+      <c r="D9" s="10">
+        <v>0</v>
+      </c>
+      <c r="E9" s="8">
+        <v>1</v>
+      </c>
+      <c r="F9" s="10">
+        <v>0</v>
+      </c>
+      <c r="G9" s="10">
+        <v>0</v>
+      </c>
+      <c r="H9" s="10">
+        <v>0</v>
+      </c>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10">
+        <v>0</v>
+      </c>
+      <c r="K9" s="10">
+        <v>0</v>
+      </c>
+      <c r="L9" s="10">
+        <v>0</v>
+      </c>
+      <c r="M9" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="A10" s="24"/>
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="8">
+        <v>17</v>
+      </c>
+      <c r="D10" s="8">
+        <v>10</v>
+      </c>
+      <c r="E10" s="6">
+        <v>177</v>
+      </c>
+      <c r="F10" s="8">
+        <v>2</v>
+      </c>
+      <c r="G10" s="10">
+        <v>0</v>
+      </c>
+      <c r="H10" s="6">
+        <v>87</v>
+      </c>
+      <c r="I10" s="6">
+        <v>38</v>
+      </c>
+      <c r="J10" s="10">
+        <v>0</v>
+      </c>
+      <c r="K10" s="8">
+        <v>13</v>
+      </c>
+      <c r="L10" s="9">
+        <v>7</v>
+      </c>
+      <c r="M10" s="8">
+        <v>2</v>
+      </c>
+      <c r="N10" s="10"/>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="A11" s="24"/>
+      <c r="B11" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="16">
-        <f t="shared" si="0"/>
+      <c r="C11" s="7">
+        <v>2</v>
+      </c>
+      <c r="D11" s="10">
+        <v>0</v>
+      </c>
+      <c r="E11" s="7">
+        <v>12</v>
+      </c>
+      <c r="F11" s="7">
+        <v>1</v>
+      </c>
+      <c r="G11" s="10">
+        <v>0</v>
+      </c>
+      <c r="H11" s="10">
+        <v>0</v>
+      </c>
+      <c r="I11" s="7">
+        <v>4</v>
+      </c>
+      <c r="J11" s="10">
+        <v>0</v>
+      </c>
+      <c r="K11" s="7">
+        <v>3</v>
+      </c>
+      <c r="L11" s="10">
+        <v>0</v>
+      </c>
+      <c r="M11" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" s="10" customFormat="1">
+      <c r="A12" s="25"/>
+      <c r="B12" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="C12" s="10">
+        <v>0</v>
+      </c>
+      <c r="D12" s="10">
+        <v>0</v>
+      </c>
+      <c r="E12" s="8">
+        <v>212</v>
+      </c>
+      <c r="F12" s="10">
+        <v>0</v>
+      </c>
+      <c r="G12" s="10">
+        <v>0</v>
+      </c>
+      <c r="H12" s="8">
+        <v>6</v>
+      </c>
+      <c r="I12" s="10">
+        <v>0</v>
+      </c>
+      <c r="J12" s="10">
+        <v>0</v>
+      </c>
+      <c r="K12" s="10">
+        <v>0</v>
+      </c>
+      <c r="L12" s="10">
+        <v>0</v>
+      </c>
+      <c r="M12" s="10">
+        <v>0</v>
+      </c>
+      <c r="N12" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" s="13" customFormat="1">
+      <c r="A13" s="26"/>
+      <c r="C13" s="16">
+        <f t="shared" ref="C13:K13" si="0">SUM(C9:C11)</f>
+        <v>19</v>
+      </c>
+      <c r="D13" s="16">
+        <f>SUM(D9:D12)</f>
         <v>10</v>
       </c>
-      <c r="E7" s="27">
-        <f t="shared" si="0"/>
-        <v>190</v>
-      </c>
-      <c r="F7" s="16">
+      <c r="E13" s="27">
+        <f>SUM(E10:E12)</f>
+        <v>401</v>
+      </c>
+      <c r="F13" s="16">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="G7" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H7" s="27">
-        <f t="shared" si="0"/>
-        <v>87</v>
-      </c>
-      <c r="I7" s="27">
-        <f>SUM(I5:I6)</f>
+      <c r="G13" s="13">
+        <f>SUM(G9:G12)</f>
+        <v>0</v>
+      </c>
+      <c r="H13" s="27">
+        <f>SUM(H9:H12)</f>
+        <v>93</v>
+      </c>
+      <c r="I13" s="27">
+        <f>SUM(I10:I11)</f>
         <v>42</v>
       </c>
-      <c r="J7" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K7" s="16">
+      <c r="J13" s="13">
+        <f>SUM(J9:J12)</f>
+        <v>0</v>
+      </c>
+      <c r="K13" s="16">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="L7" s="17">
-        <f t="shared" si="0"/>
+      <c r="L13" s="17">
+        <f>SUM(L9:L12)</f>
         <v>7</v>
       </c>
-      <c r="M7" s="16">
-        <f t="shared" si="0"/>
+      <c r="M13" s="16">
+        <f>SUM(M9:M12)</f>
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="25"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="24" t="s">
+    <row r="14" spans="1:14" s="10" customFormat="1">
+      <c r="A14" s="25"/>
+    </row>
+    <row r="15" spans="1:14">
+      <c r="A15" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B15" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C15" s="4">
         <v>20</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D15" s="4">
         <v>2</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E15" s="4">
         <v>38</v>
       </c>
-      <c r="F9" s="4">
+      <c r="F15" s="4">
         <v>16</v>
       </c>
-      <c r="G9" s="4">
+      <c r="G15" s="4">
         <v>10</v>
       </c>
-      <c r="H9" s="10">
-        <v>0</v>
-      </c>
-      <c r="I9" s="4">
+      <c r="H15" s="10">
+        <v>0</v>
+      </c>
+      <c r="I15" s="4">
         <v>6</v>
       </c>
-      <c r="J9" s="10">
-        <v>0</v>
-      </c>
-      <c r="K9" s="4">
+      <c r="J15" s="10">
+        <v>0</v>
+      </c>
+      <c r="K15" s="4">
         <v>316</v>
       </c>
-      <c r="L9" s="9">
+      <c r="L15" s="9">
         <v>6</v>
       </c>
-      <c r="M9" s="4">
+      <c r="M15" s="4">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="24"/>
-      <c r="B10" t="s">
+    <row r="16" spans="1:14">
+      <c r="A16" s="24"/>
+      <c r="B16" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="7">
+      <c r="C16" s="7">
         <v>21</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D16" s="4">
         <v>1</v>
       </c>
-      <c r="E10" s="8">
+      <c r="E16" s="8">
         <v>21</v>
       </c>
-      <c r="F10" s="7">
+      <c r="F16" s="7">
         <v>136</v>
       </c>
-      <c r="G10" s="10">
-        <v>0</v>
-      </c>
-      <c r="H10" s="8">
+      <c r="G16" s="10">
+        <v>0</v>
+      </c>
+      <c r="H16" s="8">
         <v>7</v>
       </c>
-      <c r="I10" s="4">
+      <c r="I16" s="4">
         <v>201</v>
       </c>
-      <c r="J10" s="10">
-        <v>0</v>
-      </c>
-      <c r="K10" s="4">
+      <c r="J16" s="10">
+        <v>0</v>
+      </c>
+      <c r="K16" s="4">
         <v>1</v>
       </c>
-      <c r="L10" s="10">
-        <v>0</v>
-      </c>
-      <c r="M10" s="4">
+      <c r="L16" s="10">
+        <v>0</v>
+      </c>
+      <c r="M16" s="4">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:14" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="26"/>
-      <c r="C11" s="15">
-        <f t="shared" ref="C11:M11" si="1">SUM(C9:C10)</f>
+    <row r="17" spans="1:13" s="10" customFormat="1">
+      <c r="A17" s="25"/>
+      <c r="B17" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="C17" s="10">
+        <v>0</v>
+      </c>
+      <c r="D17" s="10">
+        <v>0</v>
+      </c>
+      <c r="E17" s="10">
+        <v>5</v>
+      </c>
+      <c r="F17" s="10">
+        <v>2</v>
+      </c>
+      <c r="G17" s="10">
+        <v>0</v>
+      </c>
+      <c r="H17" s="10">
+        <v>0</v>
+      </c>
+      <c r="I17" s="10">
+        <v>0</v>
+      </c>
+      <c r="J17" s="10">
+        <v>0</v>
+      </c>
+      <c r="K17" s="10">
+        <v>3</v>
+      </c>
+      <c r="L17" s="10">
+        <v>0</v>
+      </c>
+      <c r="M17" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" s="13" customFormat="1">
+      <c r="A18" s="26"/>
+      <c r="C18" s="15">
+        <f t="shared" ref="C18:M18" si="1">SUM(C15:C16)</f>
         <v>41</v>
       </c>
-      <c r="D11" s="14">
+      <c r="D18" s="14">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="E11" s="16">
-        <f t="shared" si="1"/>
-        <v>59</v>
-      </c>
-      <c r="F11" s="15">
-        <f t="shared" si="1"/>
-        <v>152</v>
-      </c>
-      <c r="G11" s="14">
-        <f t="shared" si="1"/>
+      <c r="E18" s="16">
+        <f>SUM(E15:E17)</f>
+        <v>64</v>
+      </c>
+      <c r="F18" s="15">
+        <f>SUM(F15:F17)</f>
+        <v>154</v>
+      </c>
+      <c r="G18" s="14">
+        <f>SUM(G15:G17)</f>
         <v>10</v>
       </c>
-      <c r="H11" s="16">
+      <c r="H18" s="16">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="I11" s="14">
-        <f>SUM(I9:I10)</f>
+      <c r="I18" s="14">
+        <f>SUM(I15:I16)</f>
         <v>207</v>
       </c>
-      <c r="J11" s="13">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K11" s="14">
-        <f t="shared" si="1"/>
-        <v>317</v>
-      </c>
-      <c r="L11" s="13">
+      <c r="J18" s="13">
+        <f>SUM(J15:J17)</f>
+        <v>0</v>
+      </c>
+      <c r="K18" s="14">
+        <f>SUM(K15:K17)</f>
+        <v>320</v>
+      </c>
+      <c r="L18" s="13">
+        <f>SUM(L15:L17)</f>
+        <v>6</v>
+      </c>
+      <c r="M18" s="14">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="M11" s="14">
-        <f t="shared" si="1"/>
+    </row>
+    <row r="19" spans="1:13" s="10" customFormat="1">
+      <c r="A19" s="25"/>
+    </row>
+    <row r="20" spans="1:13">
+      <c r="A20" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20" s="10">
+        <v>0</v>
+      </c>
+      <c r="D20" s="10">
+        <v>0</v>
+      </c>
+      <c r="E20" s="4">
+        <v>4</v>
+      </c>
+      <c r="F20" s="10">
+        <v>0</v>
+      </c>
+      <c r="G20" s="10">
+        <v>0</v>
+      </c>
+      <c r="H20" s="7">
+        <v>8</v>
+      </c>
+      <c r="I20" s="7">
+        <v>2</v>
+      </c>
+      <c r="J20" s="10">
+        <v>0</v>
+      </c>
+      <c r="K20" s="7">
+        <v>3</v>
+      </c>
+      <c r="L20" s="10">
+        <v>0</v>
+      </c>
+      <c r="M20" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13">
+      <c r="A21" s="24"/>
+      <c r="B21" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21" s="10">
+        <v>0</v>
+      </c>
+      <c r="D21" s="10">
+        <v>0</v>
+      </c>
+      <c r="E21" s="7">
+        <v>11</v>
+      </c>
+      <c r="F21" s="10">
+        <v>0</v>
+      </c>
+      <c r="G21" s="10">
+        <v>0</v>
+      </c>
+      <c r="H21" s="10">
+        <v>0</v>
+      </c>
+      <c r="I21" s="10">
+        <v>0</v>
+      </c>
+      <c r="J21" s="10">
+        <v>0</v>
+      </c>
+      <c r="K21" s="10">
+        <v>0</v>
+      </c>
+      <c r="L21" s="10">
+        <v>0</v>
+      </c>
+      <c r="M21" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13">
+      <c r="A22" s="24"/>
+      <c r="B22" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22" s="5">
+        <v>135</v>
+      </c>
+      <c r="D22" s="5">
+        <v>75</v>
+      </c>
+      <c r="E22" s="5">
+        <v>127</v>
+      </c>
+      <c r="F22" s="5">
+        <v>59</v>
+      </c>
+      <c r="G22" s="10">
+        <v>0</v>
+      </c>
+      <c r="H22" s="5">
+        <v>9</v>
+      </c>
+      <c r="I22" s="8">
         <v>6</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="25"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" s="24" t="s">
+      <c r="J22" s="10">
+        <v>0</v>
+      </c>
+      <c r="K22" s="5">
         <v>24</v>
       </c>
-      <c r="B13" t="s">
-        <v>23</v>
-      </c>
-      <c r="C13" s="10">
-        <v>0</v>
-      </c>
-      <c r="D13" s="10">
-        <v>0</v>
-      </c>
-      <c r="E13" s="4">
-        <v>4</v>
-      </c>
-      <c r="F13" s="10">
-        <v>0</v>
-      </c>
-      <c r="G13" s="10">
-        <v>0</v>
-      </c>
-      <c r="H13" s="7">
+      <c r="L22" s="9">
+        <v>108</v>
+      </c>
+      <c r="M22" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" s="10" customFormat="1">
+      <c r="A23" s="25"/>
+      <c r="B23" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="C23" s="10">
+        <v>0</v>
+      </c>
+      <c r="D23" s="10">
+        <v>0</v>
+      </c>
+      <c r="E23" s="8">
+        <v>1</v>
+      </c>
+      <c r="F23" s="10">
+        <v>0</v>
+      </c>
+      <c r="G23" s="10">
+        <v>0</v>
+      </c>
+      <c r="H23" s="10">
+        <v>0</v>
+      </c>
+      <c r="I23" s="10">
+        <v>0</v>
+      </c>
+      <c r="J23" s="10">
+        <v>0</v>
+      </c>
+      <c r="K23" s="10">
+        <v>0</v>
+      </c>
+      <c r="L23" s="10">
+        <v>0</v>
+      </c>
+      <c r="M23" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" s="13" customFormat="1">
+      <c r="A24" s="26"/>
+      <c r="C24" s="28">
+        <f>SUM(C20:C23)</f>
+        <v>135</v>
+      </c>
+      <c r="D24" s="28">
+        <f>SUM(D20:D23)</f>
+        <v>75</v>
+      </c>
+      <c r="E24" s="28">
+        <f>SUM(E20:E23)</f>
+        <v>143</v>
+      </c>
+      <c r="F24" s="28">
+        <f>SUM(F20:F23)</f>
+        <v>59</v>
+      </c>
+      <c r="G24" s="13">
+        <f>SUM(G20:G23)</f>
+        <v>0</v>
+      </c>
+      <c r="H24" s="28">
+        <f t="shared" ref="H24:K24" si="2">SUM(H20:H22)</f>
+        <v>17</v>
+      </c>
+      <c r="I24" s="16">
+        <f>SUM(I20:I22)</f>
         <v>8</v>
       </c>
-      <c r="I13" s="7">
-        <v>2</v>
-      </c>
-      <c r="J13" s="10">
-        <v>0</v>
-      </c>
-      <c r="K13" s="7">
-        <v>3</v>
-      </c>
-      <c r="L13" s="10">
-        <v>0</v>
-      </c>
-      <c r="M13" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="24"/>
-      <c r="B14" t="s">
-        <v>25</v>
-      </c>
-      <c r="C14" s="10">
-        <v>0</v>
-      </c>
-      <c r="D14" s="10">
-        <v>0</v>
-      </c>
-      <c r="E14" s="7">
-        <v>11</v>
-      </c>
-      <c r="F14" s="10">
-        <v>0</v>
-      </c>
-      <c r="G14" s="10">
-        <v>0</v>
-      </c>
-      <c r="H14" s="10">
-        <v>0</v>
-      </c>
-      <c r="I14" s="10">
-        <v>0</v>
-      </c>
-      <c r="J14" s="10">
-        <v>0</v>
-      </c>
-      <c r="K14" s="10">
-        <v>0</v>
-      </c>
-      <c r="L14" s="10">
-        <v>0</v>
-      </c>
-      <c r="M14" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="24"/>
-      <c r="B15" t="s">
-        <v>26</v>
-      </c>
-      <c r="C15" s="5">
-        <v>135</v>
-      </c>
-      <c r="D15" s="5">
-        <v>75</v>
-      </c>
-      <c r="E15" s="5">
-        <v>127</v>
-      </c>
-      <c r="F15" s="5">
-        <v>59</v>
-      </c>
-      <c r="G15" s="10">
-        <v>0</v>
-      </c>
-      <c r="H15" s="5">
-        <v>9</v>
-      </c>
-      <c r="I15" s="8">
-        <v>6</v>
-      </c>
-      <c r="J15" s="10">
-        <v>0</v>
-      </c>
-      <c r="K15" s="5">
-        <v>24</v>
-      </c>
-      <c r="L15" s="9">
-        <v>108</v>
-      </c>
-      <c r="M15" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="26"/>
-      <c r="C16" s="28">
-        <f t="shared" ref="C16:M16" si="2">SUM(C13:C15)</f>
-        <v>135</v>
-      </c>
-      <c r="D16" s="28">
-        <f t="shared" si="2"/>
-        <v>75</v>
-      </c>
-      <c r="E16" s="28">
-        <f t="shared" si="2"/>
-        <v>142</v>
-      </c>
-      <c r="F16" s="28">
-        <f t="shared" si="2"/>
-        <v>59</v>
-      </c>
-      <c r="G16" s="13">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="H16" s="28">
-        <f t="shared" si="2"/>
-        <v>17</v>
-      </c>
-      <c r="I16" s="16">
-        <f>SUM(I13:I15)</f>
-        <v>8</v>
-      </c>
-      <c r="J16" s="13">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="K16" s="28">
+      <c r="J24" s="13">
+        <f>SUM(J20:J23)</f>
+        <v>0</v>
+      </c>
+      <c r="K24" s="28">
         <f t="shared" si="2"/>
         <v>27</v>
       </c>
-      <c r="L16" s="13">
-        <f t="shared" si="2"/>
+      <c r="L24" s="13">
+        <f>SUM(L20:L23)</f>
         <v>108</v>
       </c>
-      <c r="M16" s="13">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="25"/>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18" s="24" t="s">
+      <c r="M24" s="13">
+        <f>SUM(M20:M23)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" s="10" customFormat="1">
+      <c r="A25" s="25"/>
+    </row>
+    <row r="26" spans="1:13">
+      <c r="A26" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B26" t="s">
         <v>27</v>
       </c>
-      <c r="C18" s="4">
+      <c r="C26" s="4">
         <v>23</v>
       </c>
-      <c r="D18" s="4">
+      <c r="D26" s="4">
         <v>5</v>
       </c>
-      <c r="E18" s="4">
+      <c r="E26" s="4">
         <v>123</v>
       </c>
-      <c r="F18" s="10">
-        <v>0</v>
-      </c>
-      <c r="G18" s="10">
-        <v>0</v>
-      </c>
-      <c r="H18" s="10">
-        <v>0</v>
-      </c>
-      <c r="I18" s="4">
+      <c r="F26" s="10">
+        <v>0</v>
+      </c>
+      <c r="G26" s="10">
+        <v>0</v>
+      </c>
+      <c r="H26" s="10">
+        <v>0</v>
+      </c>
+      <c r="I26" s="4">
         <v>157</v>
       </c>
-      <c r="J18" s="10">
-        <v>0</v>
-      </c>
-      <c r="K18" s="4">
+      <c r="J26" s="10">
+        <v>0</v>
+      </c>
+      <c r="K26" s="4">
         <v>298</v>
       </c>
-      <c r="L18" s="4">
+      <c r="L26" s="4">
         <v>1</v>
       </c>
-      <c r="M18" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="24"/>
-      <c r="B19" t="s">
+      <c r="M26" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13">
+      <c r="A27" s="24"/>
+      <c r="B27" t="s">
         <v>31</v>
       </c>
-      <c r="C19" s="4">
+      <c r="C27" s="4">
         <v>179</v>
       </c>
-      <c r="D19" s="4">
+      <c r="D27" s="4">
         <v>1</v>
       </c>
-      <c r="E19" s="7">
+      <c r="E27" s="7">
         <v>54</v>
       </c>
-      <c r="F19" s="10">
-        <v>0</v>
-      </c>
-      <c r="G19" s="10">
-        <v>0</v>
-      </c>
-      <c r="H19" s="10">
-        <v>0</v>
-      </c>
-      <c r="I19" s="4">
+      <c r="F27" s="10">
+        <v>0</v>
+      </c>
+      <c r="G27" s="10">
+        <v>0</v>
+      </c>
+      <c r="H27" s="10">
+        <v>0</v>
+      </c>
+      <c r="I27" s="4">
         <v>10</v>
       </c>
-      <c r="J19" s="10">
-        <v>0</v>
-      </c>
-      <c r="K19" s="7">
+      <c r="J27" s="10">
+        <v>0</v>
+      </c>
+      <c r="K27" s="7">
         <v>152</v>
       </c>
-      <c r="L19" s="10">
-        <v>0</v>
-      </c>
-      <c r="M19" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C20" s="14">
-        <f t="shared" ref="C20:M20" si="3">SUM(C18:C19)</f>
-        <v>202</v>
-      </c>
-      <c r="D20" s="14">
-        <f t="shared" si="3"/>
+      <c r="L27" s="10">
+        <v>0</v>
+      </c>
+      <c r="M27" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" s="10" customFormat="1">
+      <c r="A28" s="25"/>
+      <c r="B28" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C28" s="8">
+        <v>2</v>
+      </c>
+      <c r="D28" s="10">
+        <v>0</v>
+      </c>
+      <c r="E28" s="6">
+        <v>46</v>
+      </c>
+      <c r="F28" s="10">
+        <v>0</v>
+      </c>
+      <c r="G28" s="10">
+        <v>0</v>
+      </c>
+      <c r="H28" s="8">
+        <v>21</v>
+      </c>
+      <c r="I28" s="8">
+        <v>33</v>
+      </c>
+      <c r="J28" s="10">
+        <v>0</v>
+      </c>
+      <c r="K28" s="6">
+        <v>3</v>
+      </c>
+      <c r="L28" s="10">
+        <v>0</v>
+      </c>
+      <c r="M28" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" s="13" customFormat="1">
+      <c r="C29" s="16">
+        <f>SUM(C26:C28)</f>
+        <v>204</v>
+      </c>
+      <c r="D29" s="14">
+        <f t="shared" ref="D29:K29" si="3">SUM(D26:D27)</f>
         <v>6</v>
       </c>
-      <c r="E20" s="15">
-        <f t="shared" si="3"/>
-        <v>177</v>
-      </c>
-      <c r="F20" s="13">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G20" s="13">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="H20" s="13">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="I20" s="14">
-        <f>SUM(I18:I19)</f>
+      <c r="E29" s="27">
+        <f>SUM(E26:E28)</f>
+        <v>223</v>
+      </c>
+      <c r="F29" s="13">
+        <f>SUM(F26:F28)</f>
+        <v>0</v>
+      </c>
+      <c r="G29" s="13">
+        <f>SUM(G26:G28)</f>
+        <v>0</v>
+      </c>
+      <c r="H29" s="16">
+        <f>SUM(H26:H28)</f>
+        <v>21</v>
+      </c>
+      <c r="I29" s="16">
+        <f>SUM(I26:I27)</f>
         <v>167</v>
       </c>
-      <c r="J20" s="13">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="K20" s="15">
+      <c r="J29" s="13">
+        <f>SUM(J26:J28)</f>
+        <v>0</v>
+      </c>
+      <c r="K29" s="27">
         <f t="shared" si="3"/>
         <v>450</v>
       </c>
-      <c r="L20" s="14">
-        <f t="shared" si="3"/>
+      <c r="L29" s="14">
+        <f>SUM(L26:L28)</f>
         <v>1</v>
       </c>
-      <c r="M20" s="13">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A22" s="24" t="s">
+      <c r="M29" s="13">
+        <f>SUM(M26:M28)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" s="10" customFormat="1"/>
+    <row r="31" spans="1:13">
+      <c r="A31" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B31" t="s">
         <v>52</v>
       </c>
-      <c r="C22" s="10">
-        <v>0</v>
-      </c>
-      <c r="D22" s="4">
+      <c r="C31" s="10">
+        <v>0</v>
+      </c>
+      <c r="D31" s="4">
         <v>72</v>
       </c>
-      <c r="E22" s="4">
+      <c r="E31" s="4">
         <v>8</v>
       </c>
-      <c r="F22" s="10">
-        <v>0</v>
-      </c>
-      <c r="G22" s="4">
+      <c r="F31" s="10">
+        <v>0</v>
+      </c>
+      <c r="G31" s="4">
         <v>1</v>
       </c>
-      <c r="H22" s="4">
+      <c r="H31" s="4">
         <v>56</v>
       </c>
-      <c r="I22" s="4">
+      <c r="I31" s="4">
         <v>32</v>
       </c>
-      <c r="J22" s="10">
-        <v>0</v>
-      </c>
-      <c r="K22" s="4">
+      <c r="J31" s="10">
+        <v>0</v>
+      </c>
+      <c r="K31" s="4">
         <v>3</v>
       </c>
-      <c r="L22" s="9">
+      <c r="L31" s="9">
         <v>7</v>
       </c>
-      <c r="M22" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
+      <c r="M31" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13">
+      <c r="B32" t="s">
         <v>53</v>
       </c>
-      <c r="C23" s="10">
-        <v>0</v>
-      </c>
-      <c r="D23" s="4">
+      <c r="C32" s="10">
+        <v>0</v>
+      </c>
+      <c r="D32" s="4">
         <v>7</v>
       </c>
-      <c r="E23" s="4">
+      <c r="E32" s="4">
         <v>2</v>
       </c>
-      <c r="F23" s="10">
-        <v>0</v>
-      </c>
-      <c r="G23" s="10">
-        <v>0</v>
-      </c>
-      <c r="H23" s="10">
-        <v>0</v>
-      </c>
-      <c r="I23" s="4">
+      <c r="F32" s="10">
+        <v>0</v>
+      </c>
+      <c r="G32" s="10">
+        <v>0</v>
+      </c>
+      <c r="H32" s="10">
+        <v>0</v>
+      </c>
+      <c r="I32" s="4">
         <v>4</v>
       </c>
-      <c r="J23" s="10">
-        <v>0</v>
-      </c>
-      <c r="K23" s="4">
+      <c r="J32" s="10">
+        <v>0</v>
+      </c>
+      <c r="K32" s="4">
         <v>1</v>
       </c>
-      <c r="L23" s="10">
-        <v>0</v>
-      </c>
-      <c r="M23" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C24" s="13">
-        <f t="shared" ref="C24:M24" si="4">SUM(C22:C23)</f>
-        <v>0</v>
-      </c>
-      <c r="D24" s="14">
+      <c r="L32" s="10">
+        <v>0</v>
+      </c>
+      <c r="M32" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" s="13" customFormat="1">
+      <c r="C33" s="13">
+        <f t="shared" ref="C33:M33" si="4">SUM(C31:C32)</f>
+        <v>0</v>
+      </c>
+      <c r="D33" s="14">
         <f t="shared" si="4"/>
         <v>79</v>
       </c>
-      <c r="E24" s="14">
+      <c r="E33" s="14">
         <f t="shared" si="4"/>
         <v>10</v>
       </c>
-      <c r="F24" s="13">
+      <c r="F33" s="13">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="G24" s="14">
+      <c r="G33" s="14">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="H24" s="14">
+      <c r="H33" s="14">
         <f t="shared" si="4"/>
         <v>56</v>
       </c>
-      <c r="I24" s="14">
-        <f>SUM(I22:I23)</f>
+      <c r="I33" s="14">
+        <f>SUM(I31:I32)</f>
         <v>36</v>
       </c>
-      <c r="J24" s="13">
+      <c r="J33" s="13">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="K24" s="14">
+      <c r="K33" s="14">
         <f t="shared" si="4"/>
         <v>4</v>
       </c>
-      <c r="L24" s="13">
+      <c r="L33" s="13">
         <f t="shared" si="4"/>
         <v>7</v>
       </c>
-      <c r="M24" s="13">
+      <c r="M33" s="13">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>54</v>
-      </c>
-      <c r="B26" t="s">
-        <v>55</v>
-      </c>
-      <c r="C26" s="4">
-        <v>11</v>
-      </c>
-      <c r="D26" s="10">
-        <v>0</v>
-      </c>
-      <c r="E26" s="7">
-        <v>25</v>
-      </c>
-      <c r="F26" s="10">
-        <v>0</v>
-      </c>
-      <c r="G26" s="4">
-        <v>1</v>
-      </c>
-      <c r="H26" s="10">
-        <v>0</v>
-      </c>
-      <c r="I26" s="7">
-        <v>402</v>
-      </c>
-      <c r="J26" s="10">
-        <v>0</v>
-      </c>
-      <c r="K26" s="4">
-        <v>28</v>
-      </c>
-      <c r="L26" s="10">
-        <v>0</v>
-      </c>
-      <c r="M26" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A28" s="24" t="s">
+    <row r="34" spans="1:13" s="10" customFormat="1"/>
+    <row r="35" spans="1:13">
+      <c r="A35" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B35" t="s">
         <v>57</v>
       </c>
-      <c r="C28" s="10">
-        <v>0</v>
-      </c>
-      <c r="D28" s="10">
-        <v>0</v>
-      </c>
-      <c r="E28" s="10">
-        <v>0</v>
-      </c>
-      <c r="F28" s="10">
-        <v>0</v>
-      </c>
-      <c r="G28" s="10">
-        <v>0</v>
-      </c>
-      <c r="H28" s="10">
-        <v>0</v>
-      </c>
-      <c r="I28" s="4">
+      <c r="C35" s="10">
+        <v>0</v>
+      </c>
+      <c r="D35" s="10">
+        <v>0</v>
+      </c>
+      <c r="E35" s="10">
+        <v>0</v>
+      </c>
+      <c r="F35" s="10">
+        <v>0</v>
+      </c>
+      <c r="G35" s="10">
+        <v>0</v>
+      </c>
+      <c r="H35" s="10">
+        <v>0</v>
+      </c>
+      <c r="I35" s="4">
         <v>4</v>
       </c>
-      <c r="J28" s="10">
-        <v>0</v>
-      </c>
-      <c r="K28" s="4">
+      <c r="J35" s="10">
+        <v>0</v>
+      </c>
+      <c r="K35" s="4">
         <v>3</v>
       </c>
-      <c r="L28" s="10">
-        <v>0</v>
-      </c>
-      <c r="M28" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>58</v>
-      </c>
-      <c r="B30" t="s">
-        <v>59</v>
-      </c>
-      <c r="C30" s="7">
-        <v>22</v>
-      </c>
-      <c r="D30" s="10">
-        <v>0</v>
-      </c>
-      <c r="E30" s="7">
-        <v>16</v>
-      </c>
-      <c r="F30" s="10">
-        <v>0</v>
-      </c>
-      <c r="G30" s="10">
-        <v>0</v>
-      </c>
-      <c r="H30" s="10">
-        <v>0</v>
-      </c>
-      <c r="I30" s="8">
-        <v>14</v>
-      </c>
-      <c r="J30" s="10">
-        <v>0</v>
-      </c>
-      <c r="K30" s="7">
-        <v>31</v>
-      </c>
-      <c r="L30" s="10">
-        <v>0</v>
-      </c>
-      <c r="M30" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A32" s="24" t="s">
+      <c r="L35" s="10">
+        <v>0</v>
+      </c>
+      <c r="M35" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" s="10" customFormat="1">
+      <c r="A36" s="25"/>
+    </row>
+    <row r="37" spans="1:13">
+      <c r="A37" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B37" t="s">
         <v>61</v>
       </c>
-      <c r="C32" s="4">
+      <c r="C37" s="4">
         <v>415</v>
       </c>
-      <c r="D32" s="4">
+      <c r="D37" s="4">
         <v>2708</v>
       </c>
-      <c r="E32" s="4">
+      <c r="E37" s="4">
         <v>389</v>
       </c>
-      <c r="F32" s="4">
+      <c r="F37" s="4">
         <v>6</v>
       </c>
-      <c r="G32" s="4">
+      <c r="G37" s="4">
         <v>3</v>
       </c>
-      <c r="H32" s="10">
-        <v>0</v>
-      </c>
-      <c r="I32" s="4">
+      <c r="H37" s="10">
+        <v>0</v>
+      </c>
+      <c r="I37" s="4">
         <v>621</v>
       </c>
-      <c r="J32" s="4">
+      <c r="J37" s="4">
         <v>78</v>
       </c>
-      <c r="K32" s="4">
+      <c r="K37" s="4">
         <v>226</v>
       </c>
-      <c r="L32" s="4">
+      <c r="L37" s="4">
         <v>449</v>
       </c>
-      <c r="M32" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B33" t="s">
+      <c r="M37" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13">
+      <c r="B38" t="s">
         <v>62</v>
       </c>
-      <c r="C33" s="10">
-        <v>0</v>
-      </c>
-      <c r="D33" s="10">
-        <v>0</v>
-      </c>
-      <c r="E33" s="23">
+      <c r="C38" s="10">
+        <v>0</v>
+      </c>
+      <c r="D38" s="10">
+        <v>0</v>
+      </c>
+      <c r="E38" s="23">
         <v>3</v>
       </c>
-      <c r="F33" s="10">
-        <v>0</v>
-      </c>
-      <c r="G33" s="10">
-        <v>0</v>
-      </c>
-      <c r="H33" s="10">
-        <v>0</v>
-      </c>
-      <c r="I33" s="10">
-        <v>0</v>
-      </c>
-      <c r="J33" s="10">
-        <v>0</v>
-      </c>
-      <c r="K33" s="10">
-        <v>0</v>
-      </c>
-      <c r="L33" s="10">
-        <v>0</v>
-      </c>
-      <c r="M33" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C34" s="14">
-        <f t="shared" ref="C34:M34" si="5">SUM(C32:C33)</f>
+      <c r="F38" s="10">
+        <v>0</v>
+      </c>
+      <c r="G38" s="10">
+        <v>0</v>
+      </c>
+      <c r="H38" s="10">
+        <v>0</v>
+      </c>
+      <c r="I38" s="10">
+        <v>0</v>
+      </c>
+      <c r="J38" s="10">
+        <v>0</v>
+      </c>
+      <c r="K38" s="10">
+        <v>0</v>
+      </c>
+      <c r="L38" s="10">
+        <v>0</v>
+      </c>
+      <c r="M38" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" s="13" customFormat="1">
+      <c r="C39" s="14">
+        <f t="shared" ref="C39:M39" si="5">SUM(C37:C38)</f>
         <v>415</v>
       </c>
-      <c r="D34" s="14">
+      <c r="D39" s="14">
         <f t="shared" si="5"/>
         <v>2708</v>
       </c>
-      <c r="E34" s="29">
+      <c r="E39" s="29">
         <f t="shared" si="5"/>
         <v>392</v>
       </c>
-      <c r="F34" s="14">
+      <c r="F39" s="14">
         <f t="shared" si="5"/>
         <v>6</v>
       </c>
-      <c r="G34" s="14">
+      <c r="G39" s="14">
         <f t="shared" si="5"/>
         <v>3</v>
       </c>
-      <c r="H34" s="13">
+      <c r="H39" s="13">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="I34" s="14">
-        <f>SUM(I32:I33)</f>
+      <c r="I39" s="14">
+        <f>SUM(I37:I38)</f>
         <v>621</v>
       </c>
-      <c r="J34" s="14">
+      <c r="J39" s="14">
         <f t="shared" si="5"/>
         <v>78</v>
       </c>
-      <c r="K34" s="14">
+      <c r="K39" s="14">
         <f t="shared" si="5"/>
         <v>226</v>
       </c>
-      <c r="L34" s="14">
+      <c r="L39" s="14">
         <f t="shared" si="5"/>
         <v>449</v>
       </c>
-      <c r="M34" s="13">
+      <c r="M39" s="13">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C36" s="10"/>
-      <c r="D36" s="10"/>
-      <c r="E36" s="10"/>
-      <c r="F36" s="10"/>
-      <c r="G36" s="10"/>
-      <c r="H36" s="10"/>
-      <c r="I36" s="10"/>
-      <c r="J36" s="10"/>
-      <c r="K36" s="10"/>
-      <c r="L36" s="10"/>
-      <c r="M36" s="10"/>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+    <row r="40" spans="1:13" s="13" customFormat="1">
+      <c r="E40" s="12"/>
+    </row>
+    <row r="41" spans="1:13" s="10" customFormat="1">
+      <c r="A41" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="B41" s="10" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" s="10" customFormat="1">
+      <c r="A42" s="25"/>
+      <c r="B42" s="10" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" s="10" customFormat="1">
+      <c r="A43" s="25"/>
+      <c r="B43" s="10" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" s="10" customFormat="1">
+      <c r="A44" s="25"/>
+      <c r="B44" s="10" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13">
+      <c r="B45" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" s="10" customFormat="1">
+      <c r="B46" s="10" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" s="10" customFormat="1"/>
+    <row r="48" spans="1:13">
+      <c r="A48" s="30" t="s">
+        <v>113</v>
+      </c>
+      <c r="B48" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" s="10" customFormat="1"/>
+    <row r="50" spans="1:2" s="10" customFormat="1">
+      <c r="A50" s="31" t="s">
+        <v>115</v>
+      </c>
+      <c r="B50" s="10" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="B51" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" s="30" t="s">
+        <v>118</v>
+      </c>
+      <c r="B53" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="B54" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2">
+      <c r="A57" s="30" t="s">
+        <v>121</v>
+      </c>
+      <c r="B57" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
+      <c r="B58" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
+      <c r="B59" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
+      <c r="B60" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2">
+      <c r="B61" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2">
+      <c r="B62" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2">
+      <c r="B63" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2">
+      <c r="B64" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2">
+      <c r="B65" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2">
+      <c r="B66" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2">
+      <c r="A75" s="5"/>
+      <c r="B75" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2">
+      <c r="A76" s="6"/>
+      <c r="B76" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2">
+      <c r="A77" s="8"/>
+      <c r="B77" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2">
+      <c r="A78" s="7"/>
+      <c r="B78" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2">
+      <c r="A79" s="4"/>
+      <c r="B79" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="82" spans="1:13">
+      <c r="A82" s="9"/>
+      <c r="B82" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="89" spans="1:13">
+      <c r="A89" t="s">
+        <v>54</v>
+      </c>
+      <c r="B89" t="s">
+        <v>55</v>
+      </c>
+      <c r="C89" s="4">
+        <v>11</v>
+      </c>
+      <c r="D89" s="10">
+        <v>0</v>
+      </c>
+      <c r="E89" s="7">
+        <v>25</v>
+      </c>
+      <c r="F89" s="10">
+        <v>0</v>
+      </c>
+      <c r="G89" s="4">
+        <v>1</v>
+      </c>
+      <c r="H89" s="10">
+        <v>0</v>
+      </c>
+      <c r="I89" s="7">
+        <v>402</v>
+      </c>
+      <c r="J89" s="10">
+        <v>0</v>
+      </c>
+      <c r="K89" s="4">
+        <v>28</v>
+      </c>
+      <c r="L89" s="10">
+        <v>0</v>
+      </c>
+      <c r="M89" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:13">
+      <c r="A90" s="10"/>
+      <c r="B90" s="10"/>
+      <c r="C90" s="10"/>
+      <c r="D90" s="10"/>
+      <c r="E90" s="10"/>
+      <c r="F90" s="10"/>
+      <c r="G90" s="10"/>
+      <c r="H90" s="10"/>
+      <c r="I90" s="10"/>
+      <c r="J90" s="10"/>
+      <c r="K90" s="10"/>
+      <c r="L90" s="10"/>
+      <c r="M90" s="10"/>
+    </row>
+    <row r="91" spans="1:13">
+      <c r="A91" s="10"/>
+      <c r="B91" s="10"/>
+      <c r="C91" s="10"/>
+      <c r="D91" s="10"/>
+      <c r="E91" s="10"/>
+      <c r="F91" s="10"/>
+      <c r="G91" s="10"/>
+      <c r="H91" s="10"/>
+      <c r="I91" s="10"/>
+      <c r="J91" s="10"/>
+      <c r="K91" s="10"/>
+      <c r="L91" s="10"/>
+      <c r="M91" s="10"/>
+    </row>
+    <row r="92" spans="1:13">
+      <c r="A92" t="s">
+        <v>58</v>
+      </c>
+      <c r="B92" t="s">
+        <v>59</v>
+      </c>
+      <c r="C92" s="7">
+        <v>22</v>
+      </c>
+      <c r="D92" s="10">
+        <v>0</v>
+      </c>
+      <c r="E92" s="7">
+        <v>16</v>
+      </c>
+      <c r="F92" s="10">
+        <v>0</v>
+      </c>
+      <c r="G92" s="10">
+        <v>0</v>
+      </c>
+      <c r="H92" s="10">
+        <v>0</v>
+      </c>
+      <c r="I92" s="8">
+        <v>14</v>
+      </c>
+      <c r="J92" s="10">
+        <v>0</v>
+      </c>
+      <c r="K92" s="7">
+        <v>31</v>
+      </c>
+      <c r="L92" s="10">
+        <v>0</v>
+      </c>
+      <c r="M92" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:13">
+      <c r="A93" s="10"/>
+      <c r="B93" s="10"/>
+      <c r="C93" s="10"/>
+      <c r="D93" s="10"/>
+      <c r="E93" s="10"/>
+      <c r="F93" s="10"/>
+      <c r="G93" s="10"/>
+      <c r="H93" s="10"/>
+      <c r="I93" s="10"/>
+      <c r="J93" s="10"/>
+      <c r="K93" s="10"/>
+      <c r="L93" s="10"/>
+      <c r="M93" s="10"/>
+    </row>
+    <row r="94" spans="1:13">
+      <c r="A94" s="10"/>
+      <c r="B94" s="10"/>
+      <c r="C94" s="10"/>
+      <c r="D94" s="10"/>
+      <c r="E94" s="10"/>
+      <c r="F94" s="10"/>
+      <c r="G94" s="10"/>
+      <c r="H94" s="10"/>
+      <c r="I94" s="10"/>
+      <c r="J94" s="10"/>
+      <c r="K94" s="10"/>
+      <c r="L94" s="10"/>
+      <c r="M94" s="10"/>
+    </row>
+    <row r="95" spans="1:13">
+      <c r="C95" s="10"/>
+      <c r="D95" s="10"/>
+      <c r="E95" s="10"/>
+      <c r="F95" s="10"/>
+      <c r="G95" s="10"/>
+      <c r="H95" s="10"/>
+      <c r="I95" s="10"/>
+      <c r="J95" s="10"/>
+      <c r="K95" s="10"/>
+      <c r="L95" s="10"/>
+      <c r="M95" s="10"/>
+    </row>
+    <row r="96" spans="1:13">
+      <c r="A96" t="s">
         <v>85</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B96" t="s">
         <v>84</v>
       </c>
-      <c r="C37" s="10">
-        <v>0</v>
-      </c>
-      <c r="D37" s="4">
+      <c r="C96" s="10">
+        <v>0</v>
+      </c>
+      <c r="D96" s="4">
         <v>1</v>
       </c>
-      <c r="E37" s="4">
+      <c r="E96" s="4">
         <v>8</v>
       </c>
-      <c r="F37" s="10">
-        <v>0</v>
-      </c>
-      <c r="G37" s="10">
-        <v>0</v>
-      </c>
-      <c r="H37" s="10">
-        <v>0</v>
-      </c>
-      <c r="I37" s="4">
+      <c r="F96" s="10">
+        <v>0</v>
+      </c>
+      <c r="G96" s="10">
+        <v>0</v>
+      </c>
+      <c r="H96" s="10">
+        <v>0</v>
+      </c>
+      <c r="I96" s="4">
         <v>1</v>
       </c>
-      <c r="J37" s="10">
-        <v>0</v>
-      </c>
-      <c r="K37" s="10">
-        <v>0</v>
-      </c>
-      <c r="L37" s="10">
-        <v>0</v>
-      </c>
-      <c r="M37" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C38" s="10"/>
-      <c r="D38" s="10"/>
-      <c r="E38" s="10"/>
-      <c r="F38" s="10"/>
-      <c r="G38" s="10"/>
-      <c r="H38" s="10"/>
-      <c r="I38" s="10"/>
-      <c r="J38" s="10"/>
-      <c r="K38" s="10"/>
-      <c r="L38" s="10"/>
-      <c r="M38" s="10"/>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+      <c r="J96" s="10">
+        <v>0</v>
+      </c>
+      <c r="K96" s="10">
+        <v>0</v>
+      </c>
+      <c r="L96" s="10">
+        <v>0</v>
+      </c>
+      <c r="M96" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:13">
+      <c r="C97" s="10"/>
+      <c r="D97" s="10"/>
+      <c r="E97" s="10"/>
+      <c r="F97" s="10"/>
+      <c r="G97" s="10"/>
+      <c r="H97" s="10"/>
+      <c r="I97" s="10"/>
+      <c r="J97" s="10"/>
+      <c r="K97" s="10"/>
+      <c r="L97" s="10"/>
+      <c r="M97" s="10"/>
+    </row>
+    <row r="98" spans="1:13">
+      <c r="A98" t="s">
         <v>86</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B98" t="s">
         <v>87</v>
       </c>
-      <c r="C39" s="10">
-        <v>0</v>
-      </c>
-      <c r="D39" s="7">
+      <c r="C98" s="10">
+        <v>0</v>
+      </c>
+      <c r="D98" s="7">
         <v>4</v>
       </c>
-      <c r="E39" s="7">
+      <c r="E98" s="7">
         <v>5</v>
       </c>
-      <c r="F39" s="10">
-        <v>0</v>
-      </c>
-      <c r="G39" s="10">
-        <v>0</v>
-      </c>
-      <c r="H39" s="10">
-        <v>0</v>
-      </c>
-      <c r="I39" s="7">
+      <c r="F98" s="10">
+        <v>0</v>
+      </c>
+      <c r="G98" s="10">
+        <v>0</v>
+      </c>
+      <c r="H98" s="10">
+        <v>0</v>
+      </c>
+      <c r="I98" s="7">
         <v>8</v>
       </c>
-      <c r="J39" s="10">
-        <v>0</v>
-      </c>
-      <c r="K39" s="7">
+      <c r="J98" s="10">
+        <v>0</v>
+      </c>
+      <c r="K98" s="7">
         <v>64</v>
       </c>
-      <c r="L39" s="10">
-        <v>0</v>
-      </c>
-      <c r="M39" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C40" s="10"/>
-      <c r="D40" s="10"/>
-      <c r="E40" s="10"/>
-      <c r="F40" s="10"/>
-      <c r="G40" s="10"/>
-      <c r="H40" s="10"/>
-      <c r="I40" s="10"/>
-      <c r="J40" s="10"/>
-      <c r="K40" s="10"/>
-      <c r="L40" s="10"/>
-      <c r="M40" s="10"/>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+      <c r="L98" s="10">
+        <v>0</v>
+      </c>
+      <c r="M98" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:13">
+      <c r="C99" s="10"/>
+      <c r="D99" s="10"/>
+      <c r="E99" s="10"/>
+      <c r="F99" s="10"/>
+      <c r="G99" s="10"/>
+      <c r="H99" s="10"/>
+      <c r="I99" s="10"/>
+      <c r="J99" s="10"/>
+      <c r="K99" s="10"/>
+      <c r="L99" s="10"/>
+      <c r="M99" s="10"/>
+    </row>
+    <row r="100" spans="1:13">
+      <c r="A100" t="s">
         <v>88</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B100" t="s">
         <v>89</v>
       </c>
-      <c r="C41" s="4">
+      <c r="C100" s="4">
         <v>1</v>
       </c>
-      <c r="D41" s="4">
+      <c r="D100" s="4">
         <v>2</v>
       </c>
-      <c r="E41" s="4">
+      <c r="E100" s="4">
         <v>6</v>
       </c>
-      <c r="F41" s="4">
+      <c r="F100" s="4">
         <v>2</v>
       </c>
-      <c r="G41" s="10">
-        <v>0</v>
-      </c>
-      <c r="H41" s="10">
-        <v>0</v>
-      </c>
-      <c r="I41" s="4">
+      <c r="G100" s="10">
+        <v>0</v>
+      </c>
+      <c r="H100" s="10">
+        <v>0</v>
+      </c>
+      <c r="I100" s="4">
         <v>15</v>
       </c>
-      <c r="J41" s="10">
-        <v>0</v>
-      </c>
-      <c r="K41" s="4">
+      <c r="J100" s="10">
+        <v>0</v>
+      </c>
+      <c r="K100" s="4">
         <v>19</v>
       </c>
-      <c r="L41" s="10">
-        <v>0</v>
-      </c>
-      <c r="M41" s="4">
+      <c r="L100" s="10">
+        <v>0</v>
+      </c>
+      <c r="M100" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C42" s="10"/>
-      <c r="D42" s="10"/>
-      <c r="E42" s="10"/>
-      <c r="F42" s="10"/>
-      <c r="G42" s="10"/>
-      <c r="H42" s="10"/>
-      <c r="I42" s="10"/>
-      <c r="J42" s="10"/>
-      <c r="K42" s="10"/>
-      <c r="L42" s="10"/>
-      <c r="M42" s="10"/>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+    <row r="101" spans="1:13">
+      <c r="C101" s="10"/>
+      <c r="D101" s="10"/>
+      <c r="E101" s="10"/>
+      <c r="F101" s="10"/>
+      <c r="G101" s="10"/>
+      <c r="H101" s="10"/>
+      <c r="I101" s="10"/>
+      <c r="J101" s="10"/>
+      <c r="K101" s="10"/>
+      <c r="L101" s="10"/>
+      <c r="M101" s="10"/>
+    </row>
+    <row r="102" spans="1:13">
+      <c r="A102" t="s">
         <v>91</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B102" t="s">
         <v>90</v>
       </c>
-      <c r="C43" s="10">
-        <v>0</v>
-      </c>
-      <c r="D43" s="4">
+      <c r="C102" s="10">
+        <v>0</v>
+      </c>
+      <c r="D102" s="4">
         <v>17</v>
       </c>
-      <c r="E43" s="10">
-        <v>0</v>
-      </c>
-      <c r="F43" s="10">
-        <v>0</v>
-      </c>
-      <c r="G43" s="10">
-        <v>0</v>
-      </c>
-      <c r="H43" s="10">
-        <v>0</v>
-      </c>
-      <c r="I43" s="4">
+      <c r="E102" s="10">
+        <v>0</v>
+      </c>
+      <c r="F102" s="10">
+        <v>0</v>
+      </c>
+      <c r="G102" s="10">
+        <v>0</v>
+      </c>
+      <c r="H102" s="10">
+        <v>0</v>
+      </c>
+      <c r="I102" s="4">
         <v>20</v>
       </c>
-      <c r="J43" s="10">
-        <v>0</v>
-      </c>
-      <c r="K43" s="4">
+      <c r="J102" s="10">
+        <v>0</v>
+      </c>
+      <c r="K102" s="4">
         <v>1003</v>
       </c>
-      <c r="L43" s="4">
+      <c r="L102" s="4">
         <v>14</v>
       </c>
-      <c r="M43" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B44" t="s">
+      <c r="M102" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:13">
+      <c r="B103" t="s">
         <v>92</v>
       </c>
-      <c r="C44" s="4">
+      <c r="C103" s="4">
         <v>147</v>
       </c>
-      <c r="D44" s="4">
+      <c r="D103" s="4">
         <v>7</v>
       </c>
-      <c r="E44" s="4">
+      <c r="E103" s="4">
         <v>191</v>
       </c>
-      <c r="F44" s="4">
+      <c r="F103" s="4">
         <v>37</v>
       </c>
-      <c r="G44" s="4">
+      <c r="G103" s="4">
         <v>1</v>
       </c>
-      <c r="H44" s="10">
-        <v>0</v>
-      </c>
-      <c r="I44" s="4">
+      <c r="H103" s="10">
+        <v>0</v>
+      </c>
+      <c r="I103" s="4">
         <v>157</v>
       </c>
-      <c r="J44" s="10">
-        <v>0</v>
-      </c>
-      <c r="K44" s="4">
+      <c r="J103" s="10">
+        <v>0</v>
+      </c>
+      <c r="K103" s="4">
         <v>932</v>
       </c>
-      <c r="L44" s="4">
+      <c r="L103" s="4">
         <v>40</v>
       </c>
-      <c r="M44" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C45" s="14">
-        <f>SUM(C43:C44)</f>
+      <c r="M103" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:13">
+      <c r="C104" s="14">
+        <f>SUM(C102:C103)</f>
         <v>147</v>
       </c>
-      <c r="D45" s="14">
-        <f>SUM(D43:D44)</f>
+      <c r="D104" s="14">
+        <f>SUM(D102:D103)</f>
         <v>24</v>
       </c>
-      <c r="E45" s="14">
-        <f>SUM(E43:E44)</f>
+      <c r="E104" s="14">
+        <f>SUM(E102:E103)</f>
         <v>191</v>
       </c>
-      <c r="F45" s="14">
-        <f>SUM(F43:F44)</f>
+      <c r="F104" s="14">
+        <f>SUM(F102:F103)</f>
         <v>37</v>
       </c>
-      <c r="G45" s="14">
-        <f>SUM(G43:G44)</f>
+      <c r="G104" s="14">
+        <f>SUM(G102:G103)</f>
         <v>1</v>
       </c>
-      <c r="H45" s="13">
-        <f t="shared" ref="C45:H45" si="6">SUM(H43:H44)</f>
-        <v>0</v>
-      </c>
-      <c r="I45" s="14">
-        <f>SUM(I43:I44)</f>
+      <c r="H104" s="13">
+        <f t="shared" ref="H104" si="6">SUM(H102:H103)</f>
+        <v>0</v>
+      </c>
+      <c r="I104" s="14">
+        <f>SUM(I102:I103)</f>
         <v>177</v>
       </c>
-      <c r="J45" s="13">
-        <f>SUM(J43:J44)</f>
-        <v>0</v>
-      </c>
-      <c r="K45" s="14">
-        <f>SUM(K43:K44)</f>
+      <c r="J104" s="13">
+        <f>SUM(J102:J103)</f>
+        <v>0</v>
+      </c>
+      <c r="K104" s="14">
+        <f>SUM(K102:K103)</f>
         <v>1935</v>
       </c>
-      <c r="L45" s="14">
-        <f>SUM(L43:L44)</f>
+      <c r="L104" s="14">
+        <f>SUM(L102:L103)</f>
         <v>54</v>
       </c>
-      <c r="M45" s="13">
-        <f>SUM(M43:M44)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C46" s="10"/>
-      <c r="D46" s="10"/>
-      <c r="E46" s="10"/>
-      <c r="F46" s="10"/>
-      <c r="G46" s="10"/>
-      <c r="H46" s="10"/>
-      <c r="I46" s="10"/>
-      <c r="J46" s="10"/>
-      <c r="K46" s="10"/>
-      <c r="L46" s="10"/>
-      <c r="M46" s="10"/>
-    </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+      <c r="M104" s="13">
+        <f>SUM(M102:M103)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:13">
+      <c r="C105" s="10"/>
+      <c r="D105" s="10"/>
+      <c r="E105" s="10"/>
+      <c r="F105" s="10"/>
+      <c r="G105" s="10"/>
+      <c r="H105" s="10"/>
+      <c r="I105" s="10"/>
+      <c r="J105" s="10"/>
+      <c r="K105" s="10"/>
+      <c r="L105" s="10"/>
+      <c r="M105" s="10"/>
+    </row>
+    <row r="106" spans="1:13">
+      <c r="A106" t="s">
         <v>93</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B106" t="s">
         <v>94</v>
       </c>
-      <c r="C47" s="4">
+      <c r="C106" s="4">
         <v>3</v>
       </c>
-      <c r="D47" s="10">
-        <v>0</v>
-      </c>
-      <c r="E47" s="4">
+      <c r="D106" s="10">
+        <v>0</v>
+      </c>
+      <c r="E106" s="4">
         <v>6</v>
       </c>
-      <c r="F47" s="10">
-        <v>0</v>
-      </c>
-      <c r="G47" s="10">
-        <v>0</v>
-      </c>
-      <c r="H47" s="4">
+      <c r="F106" s="10">
+        <v>0</v>
+      </c>
+      <c r="G106" s="10">
+        <v>0</v>
+      </c>
+      <c r="H106" s="4">
         <v>6</v>
       </c>
-      <c r="I47" s="4">
+      <c r="I106" s="4">
         <v>29</v>
       </c>
-      <c r="J47" s="10">
-        <v>0</v>
-      </c>
-      <c r="K47" s="4">
+      <c r="J106" s="10">
+        <v>0</v>
+      </c>
+      <c r="K106" s="4">
         <v>41</v>
       </c>
-      <c r="L47" s="4">
+      <c r="L106" s="4">
         <v>4</v>
       </c>
-      <c r="M47" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B48" t="s">
+      <c r="M106" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:13">
+      <c r="B107" t="s">
         <v>95</v>
       </c>
-      <c r="C48" s="4">
+      <c r="C107" s="4">
         <v>14</v>
       </c>
-      <c r="D48" s="4">
+      <c r="D107" s="4">
         <v>2</v>
       </c>
-      <c r="E48" s="7">
+      <c r="E107" s="7">
         <v>244</v>
       </c>
-      <c r="F48" s="10">
-        <v>0</v>
-      </c>
-      <c r="G48" s="10">
-        <v>0</v>
-      </c>
-      <c r="H48" s="7">
+      <c r="F107" s="10">
+        <v>0</v>
+      </c>
+      <c r="G107" s="10">
+        <v>0</v>
+      </c>
+      <c r="H107" s="7">
         <v>42</v>
       </c>
-      <c r="I48" s="7">
+      <c r="I107" s="7">
         <v>61</v>
       </c>
-      <c r="J48" s="10">
-        <v>0</v>
-      </c>
-      <c r="K48" s="4">
+      <c r="J107" s="10">
+        <v>0</v>
+      </c>
+      <c r="K107" s="4">
         <v>5</v>
       </c>
-      <c r="L48" s="10">
-        <v>0</v>
-      </c>
-      <c r="M48" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B49" t="s">
+      <c r="L107" s="10">
+        <v>0</v>
+      </c>
+      <c r="M107" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:13">
+      <c r="B108" t="s">
         <v>33</v>
       </c>
-      <c r="C49" s="14">
+      <c r="C108" s="14">
         <v>5</v>
       </c>
-      <c r="D49" s="14">
-        <v>0</v>
-      </c>
-      <c r="E49" s="15">
+      <c r="D108" s="14">
+        <v>0</v>
+      </c>
+      <c r="E108" s="15">
         <v>9</v>
       </c>
-      <c r="F49" s="13">
-        <v>0</v>
-      </c>
-      <c r="G49" s="13">
-        <v>0</v>
-      </c>
-      <c r="H49" s="15">
+      <c r="F108" s="13">
+        <v>0</v>
+      </c>
+      <c r="G108" s="13">
+        <v>0</v>
+      </c>
+      <c r="H108" s="15">
         <v>44</v>
       </c>
-      <c r="I49" s="15">
-        <f>SUM(I47:I48)</f>
+      <c r="I108" s="15">
+        <f>SUM(I106:I107)</f>
         <v>90</v>
       </c>
-      <c r="J49" s="13">
-        <v>0</v>
-      </c>
-      <c r="K49" s="14">
+      <c r="J108" s="13">
+        <v>0</v>
+      </c>
+      <c r="K108" s="14">
         <v>4</v>
       </c>
-      <c r="L49" s="13">
-        <v>0</v>
-      </c>
-      <c r="M49" s="13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
+      <c r="L108" s="13">
+        <v>0</v>
+      </c>
+      <c r="M108" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:13">
+      <c r="A111" t="s">
         <v>63</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B111" t="s">
         <v>64</v>
       </c>
-      <c r="C52" s="10">
+      <c r="C111" s="10">
         <v>118</v>
       </c>
-      <c r="D52" s="10">
+      <c r="D111" s="10">
         <v>420</v>
       </c>
-      <c r="E52" s="10">
+      <c r="E111" s="10">
         <v>188</v>
       </c>
-      <c r="F52" s="10">
+      <c r="F111" s="10">
         <v>2</v>
       </c>
-      <c r="G52" s="10">
+      <c r="G111" s="10">
         <v>8</v>
       </c>
-      <c r="H52" s="10">
-        <v>0</v>
-      </c>
-      <c r="I52" s="10"/>
-      <c r="J52" s="10">
-        <v>0</v>
-      </c>
-      <c r="K52" s="10">
+      <c r="H111" s="10">
+        <v>0</v>
+      </c>
+      <c r="I111" s="10"/>
+      <c r="J111" s="10">
+        <v>0</v>
+      </c>
+      <c r="K111" s="10">
         <v>297</v>
       </c>
-      <c r="L52" s="10">
+      <c r="L111" s="10">
         <v>9</v>
       </c>
-      <c r="M52" s="10">
+      <c r="M111" s="10">
         <v>2</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
+    <row r="112" spans="1:13">
+      <c r="A112" t="s">
         <v>83</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B112" t="s">
         <v>82</v>
       </c>
-      <c r="C53" s="10">
+      <c r="C112" s="10">
         <v>13</v>
       </c>
-      <c r="D53" s="10">
+      <c r="D112" s="10">
         <v>116</v>
       </c>
-      <c r="E53" s="10">
+      <c r="E112" s="10">
         <v>143</v>
       </c>
-      <c r="F53" s="10">
-        <v>0</v>
-      </c>
-      <c r="G53" s="10">
-        <v>0</v>
-      </c>
-      <c r="H53" s="10">
-        <v>0</v>
-      </c>
-      <c r="I53" s="10"/>
-      <c r="J53" s="10">
-        <v>0</v>
-      </c>
-      <c r="K53" s="10">
+      <c r="F112" s="10">
+        <v>0</v>
+      </c>
+      <c r="G112" s="10">
+        <v>0</v>
+      </c>
+      <c r="H112" s="10">
+        <v>0</v>
+      </c>
+      <c r="I112" s="10"/>
+      <c r="J112" s="10">
+        <v>0</v>
+      </c>
+      <c r="K112" s="10">
         <v>209</v>
       </c>
-      <c r="L53" s="10">
+      <c r="L112" s="10">
         <v>1</v>
       </c>
-      <c r="M53" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A60" s="5"/>
-      <c r="B60" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A61" s="6"/>
-      <c r="B61" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A62" s="8"/>
-      <c r="B62" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A63" s="7"/>
-      <c r="B63" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A64" s="4"/>
-      <c r="B64" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" s="9"/>
-      <c r="B67" t="s">
-        <v>98</v>
+      <c r="M112" s="10">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -3302,9 +4005,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -3314,9 +4022,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -3328,9 +4041,9 @@
       <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3368,7 +4081,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -3406,7 +4119,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -3444,7 +4157,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12">
       <c r="B4" t="s">
         <v>18</v>
       </c>
@@ -3479,7 +4192,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12">
       <c r="B5" t="s">
         <v>19</v>
       </c>
@@ -3514,7 +4227,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -3552,7 +4265,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12">
       <c r="B7" t="s">
         <v>22</v>
       </c>
@@ -3587,7 +4300,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -3625,7 +4338,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12">
       <c r="B9" t="s">
         <v>25</v>
       </c>
@@ -3660,7 +4373,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12">
       <c r="B10" t="s">
         <v>26</v>
       </c>
@@ -3695,7 +4408,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -3733,7 +4446,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12">
       <c r="B12" t="s">
         <v>31</v>
       </c>
@@ -3768,7 +4481,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12">
       <c r="A13" t="s">
         <v>51</v>
       </c>
@@ -3806,7 +4519,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12">
       <c r="B14" t="s">
         <v>53</v>
       </c>
@@ -3841,7 +4554,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12">
       <c r="A15" t="s">
         <v>54</v>
       </c>
@@ -3879,7 +4592,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12">
       <c r="A16" t="s">
         <v>56</v>
       </c>
@@ -3917,7 +4630,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12">
       <c r="A17" t="s">
         <v>58</v>
       </c>
@@ -3955,7 +4668,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12">
       <c r="A18" t="s">
         <v>60</v>
       </c>
@@ -3993,7 +4706,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12">
       <c r="B19" t="s">
         <v>62</v>
       </c>
@@ -4028,7 +4741,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12">
       <c r="A20" t="s">
         <v>63</v>
       </c>
@@ -4068,6 +4781,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -4079,22 +4797,22 @@
       <selection activeCell="X11" sqref="X11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" style="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" style="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.6640625" style="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.6640625" style="10" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.6640625" style="10" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.6640625" style="10" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.6640625" style="10" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.6640625" style="10" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.6640625" style="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30">
       <c r="B1" s="3" t="s">
         <v>71</v>
       </c>
@@ -4147,7 +4865,7 @@
       <c r="AC1" s="12"/>
       <c r="AD1" s="12"/>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:30">
       <c r="A2" s="3" t="s">
         <v>66</v>
       </c>
@@ -4223,7 +4941,7 @@
       <c r="AC2" s="11"/>
       <c r="AD2" s="11"/>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:30">
       <c r="A3" s="3" t="s">
         <v>65</v>
       </c>
@@ -4299,7 +5017,7 @@
       <c r="AC3" s="11"/>
       <c r="AD3" s="11"/>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:30">
       <c r="A4" s="3" t="s">
         <v>70</v>
       </c>
@@ -4375,7 +5093,7 @@
       <c r="AC4" s="11"/>
       <c r="AD4" s="11"/>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:30">
       <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
@@ -4451,7 +5169,7 @@
       <c r="AC5" s="11"/>
       <c r="AD5" s="11"/>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:30">
       <c r="A6" s="3" t="s">
         <v>9</v>
       </c>
@@ -4527,7 +5245,7 @@
       <c r="AC6" s="11"/>
       <c r="AD6" s="11"/>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:30">
       <c r="A7" s="3" t="s">
         <v>67</v>
       </c>
@@ -4603,7 +5321,7 @@
       <c r="AC7" s="11"/>
       <c r="AD7" s="11"/>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:30">
       <c r="A8" s="3" t="s">
         <v>14</v>
       </c>
@@ -4679,7 +5397,7 @@
       <c r="AC8" s="11"/>
       <c r="AD8" s="11"/>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:30">
       <c r="A9" s="3" t="s">
         <v>69</v>
       </c>
@@ -4755,7 +5473,7 @@
       <c r="AC9" s="11"/>
       <c r="AD9" s="11"/>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:30">
       <c r="A10" s="3" t="s">
         <v>68</v>
       </c>
@@ -4831,7 +5549,7 @@
       <c r="AC10" s="11"/>
       <c r="AD10" s="11"/>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:30">
       <c r="A11" s="3" t="s">
         <v>13</v>
       </c>
@@ -4907,7 +5625,7 @@
       <c r="AC11" s="11"/>
       <c r="AD11" s="11"/>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:30">
       <c r="C14" s="13"/>
       <c r="D14" s="13"/>
       <c r="E14" s="13"/>
@@ -4920,10 +5638,10 @@
       <c r="L14" s="13"/>
       <c r="M14" s="13"/>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:30">
       <c r="C16" s="13"/>
     </row>
-    <row r="17" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:15">
       <c r="C17" s="13"/>
       <c r="D17" s="13"/>
       <c r="E17" s="21"/>
@@ -4938,43 +5656,43 @@
       <c r="N17" s="21"/>
       <c r="O17" s="13"/>
     </row>
-    <row r="18" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:15">
       <c r="C18" s="13"/>
     </row>
-    <row r="19" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:15">
       <c r="C19" s="13"/>
       <c r="E19" s="21"/>
     </row>
-    <row r="20" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:15">
       <c r="C20" s="13"/>
       <c r="E20" s="21"/>
     </row>
-    <row r="21" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:15">
       <c r="C21" s="13"/>
       <c r="E21" s="11"/>
     </row>
-    <row r="22" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:15">
       <c r="C22" s="13"/>
       <c r="E22" s="21"/>
     </row>
-    <row r="23" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:15">
       <c r="C23" s="13"/>
       <c r="E23" s="21"/>
     </row>
-    <row r="24" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:15">
       <c r="C24" s="13"/>
       <c r="E24" s="21"/>
     </row>
-    <row r="25" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:15">
       <c r="E25" s="21"/>
     </row>
-    <row r="26" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:15">
       <c r="E26" s="21"/>
     </row>
-    <row r="27" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:15">
       <c r="E27" s="21"/>
     </row>
-    <row r="28" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:15">
       <c r="E28" s="21"/>
     </row>
   </sheetData>
@@ -4982,13 +5700,18 @@
     <sortCondition descending="1" ref="V2:V11"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:O20"/>
@@ -4997,17 +5720,17 @@
       <selection activeCell="B1" sqref="B1:K1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15">
       <c r="B1" s="3" t="s">
         <v>65</v>
       </c>
@@ -5043,7 +5766,7 @@
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15">
       <c r="A2" s="3" t="s">
         <v>71</v>
       </c>
@@ -5078,7 +5801,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15">
       <c r="A3" s="3" t="s">
         <v>72</v>
       </c>
@@ -5113,7 +5836,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15">
       <c r="A4" s="3" t="s">
         <v>73</v>
       </c>
@@ -5148,7 +5871,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15">
       <c r="A5" s="3" t="s">
         <v>74</v>
       </c>
@@ -5183,7 +5906,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15">
       <c r="A6" s="3" t="s">
         <v>75</v>
       </c>
@@ -5228,7 +5951,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15">
       <c r="A7" s="3" t="s">
         <v>76</v>
       </c>
@@ -5273,7 +5996,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15">
       <c r="A8" s="3" t="s">
         <v>77</v>
       </c>
@@ -5308,7 +6031,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15">
       <c r="A9" s="3" t="s">
         <v>78</v>
       </c>
@@ -5343,7 +6066,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15">
       <c r="A10" s="3" t="s">
         <v>79</v>
       </c>
@@ -5378,7 +6101,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15">
       <c r="A11" s="3" t="s">
         <v>80</v>
       </c>
@@ -5413,7 +6136,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15">
       <c r="A12" s="3" t="s">
         <v>81</v>
       </c>
@@ -5448,7 +6171,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15">
       <c r="B13" s="10"/>
       <c r="C13" s="10"/>
       <c r="D13" s="10"/>
@@ -5460,7 +6183,7 @@
       <c r="J13" s="10"/>
       <c r="K13" s="10"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15">
       <c r="B14" s="10"/>
       <c r="C14" s="10"/>
       <c r="D14" s="10"/>
@@ -5472,7 +6195,7 @@
       <c r="J14" s="10"/>
       <c r="K14" s="10"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15">
       <c r="B15" s="10"/>
       <c r="C15" s="10"/>
       <c r="D15" s="10"/>
@@ -5484,7 +6207,7 @@
       <c r="J15" s="10"/>
       <c r="K15" s="10"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15">
       <c r="B16" s="10"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
@@ -5496,7 +6219,7 @@
       <c r="J16" s="10"/>
       <c r="K16" s="10"/>
     </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:11">
       <c r="B17" s="10"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
@@ -5508,7 +6231,7 @@
       <c r="J17" s="10"/>
       <c r="K17" s="10"/>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:11">
       <c r="B18" s="10"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
@@ -5520,7 +6243,7 @@
       <c r="J18" s="10"/>
       <c r="K18" s="10"/>
     </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:11">
       <c r="B19" s="10"/>
       <c r="C19" s="10"/>
       <c r="D19" s="10"/>
@@ -5532,7 +6255,7 @@
       <c r="J19" s="10"/>
       <c r="K19" s="10"/>
     </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:11">
       <c r="B20" s="10"/>
       <c r="C20" s="10"/>
       <c r="D20" s="10"/>
@@ -5546,6 +6269,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="landscape" r:id="rId1"/>
+  <pageSetup orientation="landscape"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>